<commit_message>
Q2 new scripts added.
</commit_message>
<xml_diff>
--- a/Q2_Automation/src/main/java/com/Resources/TestData.xlsx
+++ b/Q2_Automation/src/main/java/com/Resources/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v2\TDECUProjects\Q2_Automation\src\main\java\com\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\workspace_automation\TDECUProjects\Q2_Automation\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D50475-2655-468C-A096-589778945EC1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF320E19-3523-4E14-AB06-09273C9CCF1E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="322">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -981,6 +981,24 @@
   </si>
   <si>
     <t>Cancel</t>
+  </si>
+  <si>
+    <t>user29433</t>
+  </si>
+  <si>
+    <t>Classic Checking - 294330</t>
+  </si>
+  <si>
+    <t>Work Phone</t>
+  </si>
+  <si>
+    <t>9987690987</t>
+  </si>
+  <si>
+    <t>Money Market Share Draft - 4000294332</t>
+  </si>
+  <si>
+    <t>Work Phone;Home Phone</t>
   </si>
 </sst>
 </file>
@@ -1376,7 +1394,7 @@
   <dimension ref="A1:F132"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41:F42"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2051,7 +2069,7 @@
         <v>12</v>
       </c>
       <c r="E34" t="s">
-        <v>79</v>
+        <v>316</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>15</v>
@@ -2071,7 +2089,7 @@
         <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>79</v>
+        <v>316</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>15</v>
@@ -2091,7 +2109,7 @@
         <v>12</v>
       </c>
       <c r="E36" t="s">
-        <v>79</v>
+        <v>316</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>15</v>
@@ -4158,9 +4176,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N41" sqref="N41"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4173,7 +4191,8 @@
     <col min="7" max="7" width="14.5703125" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="49.28515625" customWidth="1"/>
   </cols>
@@ -4717,16 +4736,46 @@
       <c r="A34" t="s">
         <v>299</v>
       </c>
+      <c r="J34" t="s">
+        <v>317</v>
+      </c>
+      <c r="L34" t="s">
+        <v>318</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>300</v>
       </c>
+      <c r="J35" t="s">
+        <v>317</v>
+      </c>
+      <c r="K35" t="s">
+        <v>320</v>
+      </c>
+      <c r="L35" t="s">
+        <v>318</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>305</v>
       </c>
+      <c r="J36" t="s">
+        <v>317</v>
+      </c>
+      <c r="L36" t="s">
+        <v>321</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="37" spans="1:14" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -4767,6 +4816,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated scripts and TestData.
</commit_message>
<xml_diff>
--- a/Q2_Automation/src/main/java/com/Resources/TestData.xlsx
+++ b/Q2_Automation/src/main/java/com/Resources/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\workspace_automation\TDECUProjects\Q2_Automation\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF320E19-3523-4E14-AB06-09273C9CCF1E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF0B7AB-D6A3-4458-9B88-28DE30EE1568}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="326">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -968,9 +968,6 @@
     <t>Option</t>
   </si>
   <si>
-    <t>Inquiry</t>
-  </si>
-  <si>
     <t>Print</t>
   </si>
   <si>
@@ -999,13 +996,28 @@
   </si>
   <si>
     <t>Work Phone;Home Phone</t>
+  </si>
+  <si>
+    <t>user2426526</t>
+  </si>
+  <si>
+    <t>Classic Checking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main Share </t>
+  </si>
+  <si>
+    <t>user82733</t>
+  </si>
+  <si>
+    <t>Inquire</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1036,6 +1048,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1058,7 +1076,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1076,6 +1094,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1394,7 +1413,7 @@
   <dimension ref="A1:F132"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="E41" sqref="E41:E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2069,7 +2088,7 @@
         <v>12</v>
       </c>
       <c r="E34" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>15</v>
@@ -2089,7 +2108,7 @@
         <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>15</v>
@@ -2109,7 +2128,7 @@
         <v>12</v>
       </c>
       <c r="E36" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>15</v>
@@ -2129,7 +2148,7 @@
         <v>12</v>
       </c>
       <c r="E37" t="s">
-        <v>79</v>
+        <v>315</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>15</v>
@@ -2149,7 +2168,7 @@
         <v>12</v>
       </c>
       <c r="E38" t="s">
-        <v>79</v>
+        <v>321</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>15</v>
@@ -2169,7 +2188,7 @@
         <v>12</v>
       </c>
       <c r="E39" t="s">
-        <v>79</v>
+        <v>321</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>15</v>
@@ -2189,7 +2208,7 @@
         <v>12</v>
       </c>
       <c r="E40" t="s">
-        <v>79</v>
+        <v>324</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>15</v>
@@ -2197,7 +2216,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>17</v>
@@ -2209,7 +2228,7 @@
         <v>12</v>
       </c>
       <c r="E41" t="s">
-        <v>79</v>
+        <v>324</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>15</v>
@@ -2217,7 +2236,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>17</v>
@@ -2229,7 +2248,7 @@
         <v>12</v>
       </c>
       <c r="E42" t="s">
-        <v>79</v>
+        <v>324</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>15</v>
@@ -4176,9 +4195,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K38" sqref="K38"/>
+      <selection pane="bottomLeft" activeCell="A41" sqref="A41:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4193,8 +4212,9 @@
     <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="39" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="49.28515625" customWidth="1"/>
+    <col min="14" max="14" width="49.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -4737,13 +4757,13 @@
         <v>299</v>
       </c>
       <c r="J34" t="s">
+        <v>316</v>
+      </c>
+      <c r="L34" t="s">
         <v>317</v>
       </c>
-      <c r="L34" t="s">
+      <c r="M34" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="M34" s="2" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -4751,16 +4771,16 @@
         <v>300</v>
       </c>
       <c r="J35" t="s">
+        <v>316</v>
+      </c>
+      <c r="K35" t="s">
+        <v>319</v>
+      </c>
+      <c r="L35" t="s">
         <v>317</v>
       </c>
-      <c r="K35" t="s">
-        <v>320</v>
-      </c>
-      <c r="L35" t="s">
+      <c r="M35" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="M35" s="2" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -4768,20 +4788,29 @@
         <v>305</v>
       </c>
       <c r="J36" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="L36" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>306</v>
       </c>
-      <c r="M37" s="8" t="s">
+      <c r="J37" t="s">
+        <v>322</v>
+      </c>
+      <c r="L37" t="s">
+        <v>320</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="N37" s="8" t="s">
         <v>307</v>
       </c>
     </row>
@@ -4789,29 +4818,71 @@
       <c r="A38" t="s">
         <v>308</v>
       </c>
+      <c r="L38" t="s">
+        <v>320</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>309</v>
       </c>
+      <c r="J39" t="s">
+        <v>322</v>
+      </c>
+      <c r="K39" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="L39" t="s">
+        <v>320</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>318</v>
+      </c>
       <c r="N39" t="s">
-        <v>311</v>
+        <v>325</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>313</v>
+        <v>312</v>
+      </c>
+      <c r="J40" t="s">
+        <v>322</v>
+      </c>
+      <c r="K40" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="L40" t="s">
+        <v>320</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>318</v>
       </c>
       <c r="N40" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>313</v>
+      </c>
+      <c r="J41" t="s">
+        <v>322</v>
+      </c>
+      <c r="K41" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="L41" t="s">
+        <v>320</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="N41" t="s">
         <v>314</v>
-      </c>
-      <c r="N41" t="s">
-        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Scripts modified for various components of Q2 application
</commit_message>
<xml_diff>
--- a/Q2_Automation/src/main/java/com/Resources/TestData.xlsx
+++ b/Q2_Automation/src/main/java/com/Resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECUProjects\Q2_Automation\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB59CB9A-D4F8-4C1B-B32F-546706F681EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F370522-5ED4-4248-BA4E-38CB0D878A7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="342">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1038,6 +1038,27 @@
   </si>
   <si>
     <t>Classic Checking	20276986	$199.73</t>
+  </si>
+  <si>
+    <t>Classic Checking	20276986	$200.53</t>
+  </si>
+  <si>
+    <t>20276986</t>
+  </si>
+  <si>
+    <t>734343</t>
+  </si>
+  <si>
+    <t>-69518</t>
+  </si>
+  <si>
+    <t>20276978</t>
+  </si>
+  <si>
+    <t>-1403410</t>
+  </si>
+  <si>
+    <t>Kony@567</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1124,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1125,6 +1146,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1442,8 +1464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1798,10 +1820,10 @@
         <v>12</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1818,10 +1840,10 @@
         <v>12</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>324</v>
+        <v>338</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1978,10 +2000,10 @@
         <v>12</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2358,10 +2380,10 @@
         <v>12</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>324</v>
+        <v>340</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>323</v>
+        <v>341</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2498,10 +2520,10 @@
         <v>12</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>324</v>
+        <v>340</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>323</v>
+        <v>341</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -3618,10 +3640,10 @@
         <v>12</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>324</v>
+        <v>340</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>323</v>
+        <v>341</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -4113,110 +4135,111 @@
     <hyperlink ref="F42" r:id="rId25" xr:uid="{1AEC7167-E7DC-4DC5-9CFE-5738DBC85751}"/>
     <hyperlink ref="F14" r:id="rId26" display="Kony@123" xr:uid="{E20598A3-D12E-4036-B79D-A5379225FEF9}"/>
     <hyperlink ref="F15" r:id="rId27" xr:uid="{797488D5-4874-4D11-9655-C596D784E6F5}"/>
-    <hyperlink ref="F18" r:id="rId28" display="Kony@123" xr:uid="{02DC061B-1CBA-48CB-8448-1CD95D3083EA}"/>
-    <hyperlink ref="F19" r:id="rId29" display="Kony@123" xr:uid="{F9E63619-FF09-40D3-A2E6-AB5314653268}"/>
-    <hyperlink ref="F22" r:id="rId30" display="Kony@123" xr:uid="{2DD0D6D2-8A04-45AB-A3CE-3836E08E3DA7}"/>
-    <hyperlink ref="F23" r:id="rId31" display="Kony@123" xr:uid="{F72FD78C-2C7D-44CD-9D75-5F8654FFED53}"/>
-    <hyperlink ref="F24" r:id="rId32" display="Kony@123" xr:uid="{8E933C7E-7C7E-4282-BB58-0C805634E6C3}"/>
-    <hyperlink ref="F26" r:id="rId33" display="Kony@123" xr:uid="{88A65621-5874-45A2-8984-F1B19A029D99}"/>
-    <hyperlink ref="F27" r:id="rId34" display="Kony@123" xr:uid="{C7DA0286-FD2E-4EAB-957B-4194723C1A2A}"/>
-    <hyperlink ref="F28" r:id="rId35" xr:uid="{50D4030C-F52F-443A-82CB-001795DDFC2E}"/>
-    <hyperlink ref="F29" r:id="rId36" display="Kony@123" xr:uid="{3A25612B-6BCE-4510-8223-C66C7822C71F}"/>
-    <hyperlink ref="F30" r:id="rId37" display="Kony@123" xr:uid="{C2E1D2B8-294C-4CBB-A8F4-155128347147}"/>
-    <hyperlink ref="F31" r:id="rId38" display="Kony@123" xr:uid="{5860E7F6-7EC9-4F10-9216-E8A06B35A794}"/>
-    <hyperlink ref="F32" r:id="rId39" display="Kony@123" xr:uid="{DAAC0511-A2E4-4137-8E04-5C3ED57495AD}"/>
-    <hyperlink ref="F33" r:id="rId40" display="Kony@123" xr:uid="{0F8F2825-9434-4059-84B2-BF68AC85B307}"/>
-    <hyperlink ref="F43" r:id="rId41" display="Kony@123" xr:uid="{ECC6B8B4-504C-476C-8F3C-90619201496F}"/>
-    <hyperlink ref="F44" r:id="rId42" display="Kony@123" xr:uid="{62ABA2C7-1E4C-4497-9430-285143D77BF5}"/>
-    <hyperlink ref="F45" r:id="rId43" display="Kony@123" xr:uid="{CA36AB5C-EE1E-4B0C-AACF-462859C717CF}"/>
-    <hyperlink ref="F46" r:id="rId44" display="Kony@123" xr:uid="{A51D7DE1-24A2-4419-AF67-489B6D0F14B9}"/>
-    <hyperlink ref="F47" r:id="rId45" display="Kony@123" xr:uid="{09BC58E9-6825-41D5-ABEE-996F54D90CF1}"/>
-    <hyperlink ref="F48" r:id="rId46" display="Kony@123" xr:uid="{FFC5603E-F568-4679-A667-A86A1F6E6950}"/>
-    <hyperlink ref="F49" r:id="rId47" display="Kony@123" xr:uid="{F0604CE0-185A-4493-B713-88E26D84FAF0}"/>
-    <hyperlink ref="F50" r:id="rId48" display="Kony@123" xr:uid="{B707BA4A-AA8B-4E76-8764-5D2BF5975C22}"/>
-    <hyperlink ref="F51" r:id="rId49" display="Kony@123" xr:uid="{11970BE2-F214-47A7-8C88-44EBB1E80FAF}"/>
-    <hyperlink ref="F52" r:id="rId50" display="Kony@123" xr:uid="{2B7C8356-BD2A-4006-955F-EA79E690081F}"/>
-    <hyperlink ref="F53" r:id="rId51" display="Kony@123" xr:uid="{61EFD06F-5B3B-4F09-87C8-4C5931C9047C}"/>
-    <hyperlink ref="F54" r:id="rId52" display="Kony@123" xr:uid="{E87B17A0-DD95-43C2-982F-F189F224032C}"/>
-    <hyperlink ref="F55" r:id="rId53" display="Kony@123" xr:uid="{9B8087F3-54E5-47CD-9C1E-A08F46377459}"/>
-    <hyperlink ref="F56" r:id="rId54" display="Kony@123" xr:uid="{43AF0104-E20C-41A4-A5F0-B96EFB4B1C37}"/>
-    <hyperlink ref="F57" r:id="rId55" display="Kony@123" xr:uid="{99F3B0CD-6285-4CFD-8C00-67ED4EA95A30}"/>
-    <hyperlink ref="F58" r:id="rId56" display="Kony@123" xr:uid="{F18AA546-B50E-4563-ABE8-59E5AF2CC0E2}"/>
-    <hyperlink ref="F59" r:id="rId57" display="Kony@123" xr:uid="{7306EE0B-1045-4D5E-9D4F-96E55C9097B7}"/>
-    <hyperlink ref="F60" r:id="rId58" display="Kony@123" xr:uid="{D117F9A8-22C6-41F5-A210-CBEA9FFEF2D3}"/>
-    <hyperlink ref="F61" r:id="rId59" display="Kony@123" xr:uid="{601C72CE-9736-4825-8DD5-993C2147A4C9}"/>
-    <hyperlink ref="F62" r:id="rId60" display="Kony@123" xr:uid="{0EED1D9F-BFB3-4473-BF2A-A5BC7A3FCFB6}"/>
-    <hyperlink ref="F63" r:id="rId61" display="Kony@123" xr:uid="{28F6D482-55DF-41DD-A988-2A2A32506141}"/>
-    <hyperlink ref="F64" r:id="rId62" display="Kony@123" xr:uid="{C05995A6-2557-49F4-821B-2B65E58FFA7C}"/>
-    <hyperlink ref="F65" r:id="rId63" display="Kony@123" xr:uid="{8C31F47F-AA11-4EAA-B7A9-C1F35711ACDE}"/>
-    <hyperlink ref="F66" r:id="rId64" display="Kony@123" xr:uid="{3B1DB643-4C34-4206-9579-57CC8F33B839}"/>
-    <hyperlink ref="F67" r:id="rId65" display="Kony@123" xr:uid="{91AB3591-1D4A-4E38-8FE5-AAB4E1935417}"/>
-    <hyperlink ref="F68" r:id="rId66" display="Kony@123" xr:uid="{7F2B0B62-35C5-4C65-922D-49EE44056215}"/>
-    <hyperlink ref="F69" r:id="rId67" display="Kony@123" xr:uid="{207FAAEF-09D7-40F3-A379-8ABEC15ECF4A}"/>
-    <hyperlink ref="F70" r:id="rId68" display="Kony@123" xr:uid="{B6097E8C-DDBA-4479-95B7-30A3D61476D1}"/>
-    <hyperlink ref="F71" r:id="rId69" display="Kony@123" xr:uid="{C3EED4F6-81DC-456C-B78A-F00631A92AF1}"/>
-    <hyperlink ref="F72" r:id="rId70" display="Kony@123" xr:uid="{6889B3FD-236F-4A54-AFCA-0884565378C9}"/>
-    <hyperlink ref="F73" r:id="rId71" display="Kony@123" xr:uid="{96829630-6B12-4619-B58B-900790AB2D8C}"/>
-    <hyperlink ref="F74" r:id="rId72" display="Kony@123" xr:uid="{4FCD289B-5FFD-478D-B4CA-6E2208E33844}"/>
-    <hyperlink ref="F75" r:id="rId73" display="Kony@123" xr:uid="{D9296A31-DC6F-4C6F-9CDB-AC84176EDE18}"/>
-    <hyperlink ref="F76" r:id="rId74" display="Kony@123" xr:uid="{F5566EFA-DAD3-4A73-B8F8-33B6E99DACF4}"/>
-    <hyperlink ref="F77" r:id="rId75" display="Kony@123" xr:uid="{1F4DA024-92EB-493D-9705-5E7AA901CEEC}"/>
-    <hyperlink ref="F78" r:id="rId76" display="Kony@123" xr:uid="{59406998-B10C-4278-8247-E46C691AE044}"/>
-    <hyperlink ref="F79" r:id="rId77" display="Kony@123" xr:uid="{49CFAF99-32F4-487A-8C7A-9AE0BB4ABD45}"/>
-    <hyperlink ref="F80" r:id="rId78" display="Kony@123" xr:uid="{BD0939B4-FC13-4AA6-B4A3-7CEAA9743D4A}"/>
-    <hyperlink ref="F81" r:id="rId79" display="Kony@123" xr:uid="{D3CD5A29-411B-4E09-8352-6C8522164A53}"/>
-    <hyperlink ref="F84" r:id="rId80" display="Kony@123" xr:uid="{E0DA70EE-A882-4587-AF63-B58F8DA48D6B}"/>
-    <hyperlink ref="F85" r:id="rId81" display="Kony@123" xr:uid="{EFA23262-BD6A-4859-88B7-12FB2C5C2368}"/>
-    <hyperlink ref="F86" r:id="rId82" display="Kony@123" xr:uid="{B9DA6CC4-5704-4A32-80B5-B2518451341D}"/>
-    <hyperlink ref="F89" r:id="rId83" display="Kony@123" xr:uid="{BFAFDF5A-2C79-4496-B7D1-383987AB5D48}"/>
-    <hyperlink ref="F90" r:id="rId84" display="Kony@123" xr:uid="{EBD95D4A-0E92-4ADE-9C6F-08A98F31003A}"/>
-    <hyperlink ref="F91" r:id="rId85" display="Kony@123" xr:uid="{CA9B003C-7272-455D-A1B2-88B8573357E5}"/>
-    <hyperlink ref="F92" r:id="rId86" display="Kony@123" xr:uid="{F4F5213E-D068-407C-9949-C43C6EEF2F46}"/>
-    <hyperlink ref="F96" r:id="rId87" display="Kony@123" xr:uid="{D627F46D-FB68-49A1-8615-B6950665BAF4}"/>
-    <hyperlink ref="F97" r:id="rId88" display="Kony@123" xr:uid="{00F1D0DF-5FE3-4ABB-893D-A37E52ECC621}"/>
-    <hyperlink ref="F98" r:id="rId89" display="Kony@123" xr:uid="{CD792B90-5575-4831-92E5-915207923D76}"/>
-    <hyperlink ref="F99" r:id="rId90" display="Kony@123" xr:uid="{76CFE16A-650C-439B-9C22-C68E0B0B267C}"/>
-    <hyperlink ref="F100" r:id="rId91" display="Kony@123" xr:uid="{A00B3C81-DB06-4191-8BFA-EE577D6701B3}"/>
-    <hyperlink ref="F107" r:id="rId92" display="Kony@123" xr:uid="{FB7EBC02-45B8-46D5-9E77-F69157ED3B73}"/>
-    <hyperlink ref="F108" r:id="rId93" display="Kony@123" xr:uid="{91CF6712-347A-4D29-B1B2-E64D0BE4D287}"/>
-    <hyperlink ref="F109" r:id="rId94" display="Kony@123" xr:uid="{F4F66B71-AEB5-43B6-8514-CE3476D807E4}"/>
-    <hyperlink ref="F110" r:id="rId95" display="Kony@123" xr:uid="{B7EC3C8A-775B-4BC1-8C19-991F98683E67}"/>
-    <hyperlink ref="F111" r:id="rId96" display="Kony@123" xr:uid="{E3AD6D4F-9B42-4529-A7C4-8E7686BEEC64}"/>
-    <hyperlink ref="F112" r:id="rId97" display="Kony@123" xr:uid="{17DECF45-DBF0-4563-BA0A-CD3D3FF6E72A}"/>
-    <hyperlink ref="F113" r:id="rId98" display="Kony@123" xr:uid="{74E6133A-5984-446E-9AA7-D829434D955D}"/>
-    <hyperlink ref="F114" r:id="rId99" display="Kony@123" xr:uid="{35D315E7-C289-4A17-9DD8-F83E1A9B2F46}"/>
-    <hyperlink ref="F115" r:id="rId100" display="Kony@123" xr:uid="{A2CC87E9-2252-43BB-97E1-082355B40DF0}"/>
-    <hyperlink ref="F116" r:id="rId101" display="Kony@123" xr:uid="{2D34241B-CE91-4101-8D20-5C35A0C31186}"/>
-    <hyperlink ref="F117" r:id="rId102" display="Kony@123" xr:uid="{E85D5C55-6C66-44D1-8EE8-FF75DDE4289F}"/>
-    <hyperlink ref="F118" r:id="rId103" display="Kony@123" xr:uid="{1D0D0690-E08E-42CF-B7C4-47A6E2A013B0}"/>
-    <hyperlink ref="F119" r:id="rId104" display="Kony@123" xr:uid="{10553AA3-7C1D-48C2-97B4-01987B6CF4B2}"/>
-    <hyperlink ref="F120" r:id="rId105" display="Kony@123" xr:uid="{2BA1CF86-E059-4693-A118-EC666FB9EDCB}"/>
-    <hyperlink ref="F121" r:id="rId106" display="Kony@123" xr:uid="{D58D3CEB-BE9A-421C-A948-D1CED862519C}"/>
-    <hyperlink ref="F122" r:id="rId107" display="Kony@123" xr:uid="{00D16CB0-272E-41E7-A8AB-235E01DB1883}"/>
-    <hyperlink ref="F123" r:id="rId108" display="Kony@123" xr:uid="{577EDD20-C8A2-4861-9251-5B00B7827C4B}"/>
-    <hyperlink ref="F128" r:id="rId109" display="Kony@123" xr:uid="{10D566E7-7697-43E4-BABF-C3FAD44D8AB6}"/>
-    <hyperlink ref="F129" r:id="rId110" display="Kony@123" xr:uid="{E1A46BAA-9D3D-42AC-BB3E-96A169AAAFEA}"/>
-    <hyperlink ref="F130" r:id="rId111" display="Kony@123" xr:uid="{3BC87084-E1A8-44C3-8A98-D632014FAB47}"/>
-    <hyperlink ref="F131" r:id="rId112" display="Kony@123" xr:uid="{2E18C221-46CD-4596-98DD-7F32DE9FE176}"/>
-    <hyperlink ref="F132" r:id="rId113" display="Kony@123" xr:uid="{36FFA7B7-D5E3-4261-BC25-1DCA79A972F7}"/>
-    <hyperlink ref="F2" r:id="rId114" display="Kony@123" xr:uid="{E78EB2EC-C5A6-4ADB-92B1-30AF16E9A9DE}"/>
-    <hyperlink ref="F3" r:id="rId115" display="Kony@123" xr:uid="{32CAA502-4931-476C-8000-ED184140DE4F}"/>
-    <hyperlink ref="F4" r:id="rId116" display="Kony@123" xr:uid="{69A9D0A6-60E4-4D3D-B29D-B95BF93E4981}"/>
-    <hyperlink ref="F5" r:id="rId117" display="Kony@123" xr:uid="{5091E8A5-7013-46C8-BC8B-B86558157BCD}"/>
-    <hyperlink ref="F6" r:id="rId118" display="Kony@123" xr:uid="{B74D3980-6E01-42D1-901D-BD12D50A30AE}"/>
-    <hyperlink ref="F7" r:id="rId119" display="Kony@123" xr:uid="{57721B33-B3BD-4051-8169-2C28B6D4B305}"/>
-    <hyperlink ref="F8" r:id="rId120" display="Kony@123" xr:uid="{EF7BC8C9-987F-44F5-B88C-66BD0FA06576}"/>
-    <hyperlink ref="F9" r:id="rId121" display="Kony@123" xr:uid="{9DF6059A-CD9E-4E25-9562-2E03B723557D}"/>
-    <hyperlink ref="F10" r:id="rId122" display="Kony@123" xr:uid="{7DD10A29-4028-49DA-94DA-13A8D33212A9}"/>
-    <hyperlink ref="F12" r:id="rId123" display="Kony@123" xr:uid="{31BED371-F74D-4171-998E-012849031283}"/>
-    <hyperlink ref="F125" r:id="rId124" xr:uid="{FFA89B18-B260-4132-B594-3EB3B642A598}"/>
-    <hyperlink ref="F25" r:id="rId125" xr:uid="{90BC1D2D-3D72-4AB6-A40A-21B53DD1F5D2}"/>
-    <hyperlink ref="F126" r:id="rId126" xr:uid="{69E5115A-2CB4-48F5-B13D-808D09C339F9}"/>
-    <hyperlink ref="F127" r:id="rId127" xr:uid="{1BD2B876-AC66-4F0E-A35D-F07F90DCF42E}"/>
-    <hyperlink ref="B28" r:id="rId128" location="/login" xr:uid="{6C13B286-E7D4-49E1-B5B5-8761B5642189}"/>
+    <hyperlink ref="F19" r:id="rId28" xr:uid="{F9E63619-FF09-40D3-A2E6-AB5314653268}"/>
+    <hyperlink ref="F22" r:id="rId29" display="Kony@123" xr:uid="{2DD0D6D2-8A04-45AB-A3CE-3836E08E3DA7}"/>
+    <hyperlink ref="F23" r:id="rId30" display="Kony@123" xr:uid="{F72FD78C-2C7D-44CD-9D75-5F8654FFED53}"/>
+    <hyperlink ref="F24" r:id="rId31" display="Kony@123" xr:uid="{8E933C7E-7C7E-4282-BB58-0C805634E6C3}"/>
+    <hyperlink ref="F26" r:id="rId32" display="Kony@123" xr:uid="{88A65621-5874-45A2-8984-F1B19A029D99}"/>
+    <hyperlink ref="F28" r:id="rId33" xr:uid="{50D4030C-F52F-443A-82CB-001795DDFC2E}"/>
+    <hyperlink ref="F29" r:id="rId34" display="Kony@123" xr:uid="{3A25612B-6BCE-4510-8223-C66C7822C71F}"/>
+    <hyperlink ref="F30" r:id="rId35" display="Kony@123" xr:uid="{C2E1D2B8-294C-4CBB-A8F4-155128347147}"/>
+    <hyperlink ref="F31" r:id="rId36" display="Kony@123" xr:uid="{5860E7F6-7EC9-4F10-9216-E8A06B35A794}"/>
+    <hyperlink ref="F32" r:id="rId37" display="Kony@123" xr:uid="{DAAC0511-A2E4-4137-8E04-5C3ED57495AD}"/>
+    <hyperlink ref="F33" r:id="rId38" display="Kony@123" xr:uid="{0F8F2825-9434-4059-84B2-BF68AC85B307}"/>
+    <hyperlink ref="F43" r:id="rId39" display="Kony@123" xr:uid="{ECC6B8B4-504C-476C-8F3C-90619201496F}"/>
+    <hyperlink ref="F44" r:id="rId40" display="Kony@123" xr:uid="{62ABA2C7-1E4C-4497-9430-285143D77BF5}"/>
+    <hyperlink ref="F45" r:id="rId41" display="Kony@123" xr:uid="{CA36AB5C-EE1E-4B0C-AACF-462859C717CF}"/>
+    <hyperlink ref="F46" r:id="rId42" xr:uid="{A51D7DE1-24A2-4419-AF67-489B6D0F14B9}"/>
+    <hyperlink ref="F47" r:id="rId43" display="Kony@123" xr:uid="{09BC58E9-6825-41D5-ABEE-996F54D90CF1}"/>
+    <hyperlink ref="F48" r:id="rId44" display="Kony@123" xr:uid="{FFC5603E-F568-4679-A667-A86A1F6E6950}"/>
+    <hyperlink ref="F49" r:id="rId45" display="Kony@123" xr:uid="{F0604CE0-185A-4493-B713-88E26D84FAF0}"/>
+    <hyperlink ref="F50" r:id="rId46" display="Kony@123" xr:uid="{B707BA4A-AA8B-4E76-8764-5D2BF5975C22}"/>
+    <hyperlink ref="F51" r:id="rId47" display="Kony@123" xr:uid="{11970BE2-F214-47A7-8C88-44EBB1E80FAF}"/>
+    <hyperlink ref="F52" r:id="rId48" display="Kony@123" xr:uid="{2B7C8356-BD2A-4006-955F-EA79E690081F}"/>
+    <hyperlink ref="F53" r:id="rId49" xr:uid="{61EFD06F-5B3B-4F09-87C8-4C5931C9047C}"/>
+    <hyperlink ref="F54" r:id="rId50" display="Kony@123" xr:uid="{E87B17A0-DD95-43C2-982F-F189F224032C}"/>
+    <hyperlink ref="F55" r:id="rId51" display="Kony@123" xr:uid="{9B8087F3-54E5-47CD-9C1E-A08F46377459}"/>
+    <hyperlink ref="F56" r:id="rId52" display="Kony@123" xr:uid="{43AF0104-E20C-41A4-A5F0-B96EFB4B1C37}"/>
+    <hyperlink ref="F57" r:id="rId53" display="Kony@123" xr:uid="{99F3B0CD-6285-4CFD-8C00-67ED4EA95A30}"/>
+    <hyperlink ref="F58" r:id="rId54" display="Kony@123" xr:uid="{F18AA546-B50E-4563-ABE8-59E5AF2CC0E2}"/>
+    <hyperlink ref="F59" r:id="rId55" display="Kony@123" xr:uid="{7306EE0B-1045-4D5E-9D4F-96E55C9097B7}"/>
+    <hyperlink ref="F60" r:id="rId56" display="Kony@123" xr:uid="{D117F9A8-22C6-41F5-A210-CBEA9FFEF2D3}"/>
+    <hyperlink ref="F61" r:id="rId57" display="Kony@123" xr:uid="{601C72CE-9736-4825-8DD5-993C2147A4C9}"/>
+    <hyperlink ref="F62" r:id="rId58" display="Kony@123" xr:uid="{0EED1D9F-BFB3-4473-BF2A-A5BC7A3FCFB6}"/>
+    <hyperlink ref="F63" r:id="rId59" display="Kony@123" xr:uid="{28F6D482-55DF-41DD-A988-2A2A32506141}"/>
+    <hyperlink ref="F64" r:id="rId60" display="Kony@123" xr:uid="{C05995A6-2557-49F4-821B-2B65E58FFA7C}"/>
+    <hyperlink ref="F66" r:id="rId61" display="Kony@123" xr:uid="{3B1DB643-4C34-4206-9579-57CC8F33B839}"/>
+    <hyperlink ref="F67" r:id="rId62" display="Kony@123" xr:uid="{91AB3591-1D4A-4E38-8FE5-AAB4E1935417}"/>
+    <hyperlink ref="F68" r:id="rId63" display="Kony@123" xr:uid="{7F2B0B62-35C5-4C65-922D-49EE44056215}"/>
+    <hyperlink ref="F69" r:id="rId64" display="Kony@123" xr:uid="{207FAAEF-09D7-40F3-A379-8ABEC15ECF4A}"/>
+    <hyperlink ref="F70" r:id="rId65" display="Kony@123" xr:uid="{B6097E8C-DDBA-4479-95B7-30A3D61476D1}"/>
+    <hyperlink ref="F71" r:id="rId66" display="Kony@123" xr:uid="{C3EED4F6-81DC-456C-B78A-F00631A92AF1}"/>
+    <hyperlink ref="F72" r:id="rId67" display="Kony@123" xr:uid="{6889B3FD-236F-4A54-AFCA-0884565378C9}"/>
+    <hyperlink ref="F73" r:id="rId68" display="Kony@123" xr:uid="{96829630-6B12-4619-B58B-900790AB2D8C}"/>
+    <hyperlink ref="F74" r:id="rId69" display="Kony@123" xr:uid="{4FCD289B-5FFD-478D-B4CA-6E2208E33844}"/>
+    <hyperlink ref="F75" r:id="rId70" display="Kony@123" xr:uid="{D9296A31-DC6F-4C6F-9CDB-AC84176EDE18}"/>
+    <hyperlink ref="F76" r:id="rId71" display="Kony@123" xr:uid="{F5566EFA-DAD3-4A73-B8F8-33B6E99DACF4}"/>
+    <hyperlink ref="F77" r:id="rId72" display="Kony@123" xr:uid="{1F4DA024-92EB-493D-9705-5E7AA901CEEC}"/>
+    <hyperlink ref="F78" r:id="rId73" display="Kony@123" xr:uid="{59406998-B10C-4278-8247-E46C691AE044}"/>
+    <hyperlink ref="F79" r:id="rId74" display="Kony@123" xr:uid="{49CFAF99-32F4-487A-8C7A-9AE0BB4ABD45}"/>
+    <hyperlink ref="F80" r:id="rId75" display="Kony@123" xr:uid="{BD0939B4-FC13-4AA6-B4A3-7CEAA9743D4A}"/>
+    <hyperlink ref="F81" r:id="rId76" display="Kony@123" xr:uid="{D3CD5A29-411B-4E09-8352-6C8522164A53}"/>
+    <hyperlink ref="F84" r:id="rId77" display="Kony@123" xr:uid="{E0DA70EE-A882-4587-AF63-B58F8DA48D6B}"/>
+    <hyperlink ref="F85" r:id="rId78" display="Kony@123" xr:uid="{EFA23262-BD6A-4859-88B7-12FB2C5C2368}"/>
+    <hyperlink ref="F86" r:id="rId79" display="Kony@123" xr:uid="{B9DA6CC4-5704-4A32-80B5-B2518451341D}"/>
+    <hyperlink ref="F89" r:id="rId80" display="Kony@123" xr:uid="{BFAFDF5A-2C79-4496-B7D1-383987AB5D48}"/>
+    <hyperlink ref="F90" r:id="rId81" display="Kony@123" xr:uid="{EBD95D4A-0E92-4ADE-9C6F-08A98F31003A}"/>
+    <hyperlink ref="F91" r:id="rId82" display="Kony@123" xr:uid="{CA9B003C-7272-455D-A1B2-88B8573357E5}"/>
+    <hyperlink ref="F92" r:id="rId83" display="Kony@123" xr:uid="{F4F5213E-D068-407C-9949-C43C6EEF2F46}"/>
+    <hyperlink ref="F96" r:id="rId84" display="Kony@123" xr:uid="{D627F46D-FB68-49A1-8615-B6950665BAF4}"/>
+    <hyperlink ref="F97" r:id="rId85" display="Kony@123" xr:uid="{00F1D0DF-5FE3-4ABB-893D-A37E52ECC621}"/>
+    <hyperlink ref="F98" r:id="rId86" display="Kony@123" xr:uid="{CD792B90-5575-4831-92E5-915207923D76}"/>
+    <hyperlink ref="F99" r:id="rId87" display="Kony@123" xr:uid="{76CFE16A-650C-439B-9C22-C68E0B0B267C}"/>
+    <hyperlink ref="F100" r:id="rId88" display="Kony@123" xr:uid="{A00B3C81-DB06-4191-8BFA-EE577D6701B3}"/>
+    <hyperlink ref="F107" r:id="rId89" display="Kony@123" xr:uid="{FB7EBC02-45B8-46D5-9E77-F69157ED3B73}"/>
+    <hyperlink ref="F108" r:id="rId90" display="Kony@123" xr:uid="{91CF6712-347A-4D29-B1B2-E64D0BE4D287}"/>
+    <hyperlink ref="F109" r:id="rId91" xr:uid="{F4F66B71-AEB5-43B6-8514-CE3476D807E4}"/>
+    <hyperlink ref="F110" r:id="rId92" display="Kony@123" xr:uid="{B7EC3C8A-775B-4BC1-8C19-991F98683E67}"/>
+    <hyperlink ref="F111" r:id="rId93" display="Kony@123" xr:uid="{E3AD6D4F-9B42-4529-A7C4-8E7686BEEC64}"/>
+    <hyperlink ref="F112" r:id="rId94" display="Kony@123" xr:uid="{17DECF45-DBF0-4563-BA0A-CD3D3FF6E72A}"/>
+    <hyperlink ref="F113" r:id="rId95" display="Kony@123" xr:uid="{74E6133A-5984-446E-9AA7-D829434D955D}"/>
+    <hyperlink ref="F114" r:id="rId96" display="Kony@123" xr:uid="{35D315E7-C289-4A17-9DD8-F83E1A9B2F46}"/>
+    <hyperlink ref="F115" r:id="rId97" display="Kony@123" xr:uid="{A2CC87E9-2252-43BB-97E1-082355B40DF0}"/>
+    <hyperlink ref="F116" r:id="rId98" display="Kony@123" xr:uid="{2D34241B-CE91-4101-8D20-5C35A0C31186}"/>
+    <hyperlink ref="F117" r:id="rId99" display="Kony@123" xr:uid="{E85D5C55-6C66-44D1-8EE8-FF75DDE4289F}"/>
+    <hyperlink ref="F118" r:id="rId100" display="Kony@123" xr:uid="{1D0D0690-E08E-42CF-B7C4-47A6E2A013B0}"/>
+    <hyperlink ref="F119" r:id="rId101" display="Kony@123" xr:uid="{10553AA3-7C1D-48C2-97B4-01987B6CF4B2}"/>
+    <hyperlink ref="F120" r:id="rId102" display="Kony@123" xr:uid="{2BA1CF86-E059-4693-A118-EC666FB9EDCB}"/>
+    <hyperlink ref="F121" r:id="rId103" display="Kony@123" xr:uid="{D58D3CEB-BE9A-421C-A948-D1CED862519C}"/>
+    <hyperlink ref="F122" r:id="rId104" display="Kony@123" xr:uid="{00D16CB0-272E-41E7-A8AB-235E01DB1883}"/>
+    <hyperlink ref="F123" r:id="rId105" display="Kony@123" xr:uid="{577EDD20-C8A2-4861-9251-5B00B7827C4B}"/>
+    <hyperlink ref="F128" r:id="rId106" display="Kony@123" xr:uid="{10D566E7-7697-43E4-BABF-C3FAD44D8AB6}"/>
+    <hyperlink ref="F129" r:id="rId107" display="Kony@123" xr:uid="{E1A46BAA-9D3D-42AC-BB3E-96A169AAAFEA}"/>
+    <hyperlink ref="F130" r:id="rId108" display="Kony@123" xr:uid="{3BC87084-E1A8-44C3-8A98-D632014FAB47}"/>
+    <hyperlink ref="F131" r:id="rId109" display="Kony@123" xr:uid="{2E18C221-46CD-4596-98DD-7F32DE9FE176}"/>
+    <hyperlink ref="F132" r:id="rId110" display="Kony@123" xr:uid="{36FFA7B7-D5E3-4261-BC25-1DCA79A972F7}"/>
+    <hyperlink ref="F2" r:id="rId111" display="Kony@123" xr:uid="{E78EB2EC-C5A6-4ADB-92B1-30AF16E9A9DE}"/>
+    <hyperlink ref="F3" r:id="rId112" display="Kony@123" xr:uid="{32CAA502-4931-476C-8000-ED184140DE4F}"/>
+    <hyperlink ref="F4" r:id="rId113" display="Kony@123" xr:uid="{69A9D0A6-60E4-4D3D-B29D-B95BF93E4981}"/>
+    <hyperlink ref="F5" r:id="rId114" display="Kony@123" xr:uid="{5091E8A5-7013-46C8-BC8B-B86558157BCD}"/>
+    <hyperlink ref="F6" r:id="rId115" display="Kony@123" xr:uid="{B74D3980-6E01-42D1-901D-BD12D50A30AE}"/>
+    <hyperlink ref="F7" r:id="rId116" display="Kony@123" xr:uid="{57721B33-B3BD-4051-8169-2C28B6D4B305}"/>
+    <hyperlink ref="F8" r:id="rId117" display="Kony@123" xr:uid="{EF7BC8C9-987F-44F5-B88C-66BD0FA06576}"/>
+    <hyperlink ref="F9" r:id="rId118" display="Kony@123" xr:uid="{9DF6059A-CD9E-4E25-9562-2E03B723557D}"/>
+    <hyperlink ref="F10" r:id="rId119" display="Kony@123" xr:uid="{7DD10A29-4028-49DA-94DA-13A8D33212A9}"/>
+    <hyperlink ref="F12" r:id="rId120" display="Kony@123" xr:uid="{31BED371-F74D-4171-998E-012849031283}"/>
+    <hyperlink ref="F125" r:id="rId121" xr:uid="{FFA89B18-B260-4132-B594-3EB3B642A598}"/>
+    <hyperlink ref="F25" r:id="rId122" xr:uid="{90BC1D2D-3D72-4AB6-A40A-21B53DD1F5D2}"/>
+    <hyperlink ref="F126" r:id="rId123" xr:uid="{69E5115A-2CB4-48F5-B13D-808D09C339F9}"/>
+    <hyperlink ref="F127" r:id="rId124" xr:uid="{1BD2B876-AC66-4F0E-A35D-F07F90DCF42E}"/>
+    <hyperlink ref="B28" r:id="rId125" location="/login" xr:uid="{6C13B286-E7D4-49E1-B5B5-8761B5642189}"/>
+    <hyperlink ref="F18" r:id="rId126" xr:uid="{41A3A24C-8B2B-4D97-8F9C-4B1C383F74A6}"/>
+    <hyperlink ref="B18" r:id="rId127" location="/login" xr:uid="{258BC967-6692-4289-9579-239320C007CA}"/>
+    <hyperlink ref="F27" r:id="rId128" xr:uid="{B73F26A9-67C2-485D-B134-1A8492A59172}"/>
+    <hyperlink ref="F65" r:id="rId129" display="Kony@123" xr:uid="{8C31F47F-AA11-4EAA-B7A9-C1F35711ACDE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId129"/>
+  <pageSetup orientation="portrait" r:id="rId130"/>
 </worksheet>
 </file>
 
@@ -4224,9 +4247,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O8" sqref="O8"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4403,10 +4426,10 @@
         <v>37</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>335</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>20</v>
+        <v>335</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>216</v>
@@ -4420,10 +4443,10 @@
         <v>39</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>339</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>20</v>
+        <v>337</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s">
@@ -4472,11 +4495,11 @@
       <c r="A13" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>29</v>
+      <c r="B13" s="13" t="s">
+        <v>336</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>337</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" t="s">
@@ -5177,7 +5200,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5185,7 +5208,7 @@
     <col min="1" max="1" width="46.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="23.5703125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="13.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>

</xml_diff>

<commit_message>
Ädded more modified scripts of Transfers
</commit_message>
<xml_diff>
--- a/Q2_Automation/src/main/java/com/Resources/TestData.xlsx
+++ b/Q2_Automation/src/main/java/com/Resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v6_Project_updates\TDECUProjects\Q2_Automation\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BA61FB-B761-4802-A281-FEB8907F5499}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0052FF7E-BC73-43A2-83E5-C89975016A49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="325">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1013,6 +1013,9 @@
   </si>
   <si>
     <t>-1403410</t>
+  </si>
+  <si>
+    <t>1st day of the month</t>
   </si>
 </sst>
 </file>
@@ -1414,8 +1417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView topLeftCell="A101" zoomScale="80" workbookViewId="0">
-      <selection activeCell="E118" sqref="E118:F118"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="80" workbookViewId="0">
+      <selection activeCell="F118" sqref="F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4163,7 +4166,7 @@
     <hyperlink ref="F115" r:id="rId103" display="Kony@123" xr:uid="{C2E080EC-EE6D-4EBC-B2BE-24781ADB0442}"/>
     <hyperlink ref="F116" r:id="rId104" display="Kony@123" xr:uid="{3187464A-9470-4D02-9F1E-52C4C055ECF2}"/>
     <hyperlink ref="F117" r:id="rId105" display="Kony@123" xr:uid="{159DA2BB-A519-4242-B0EA-1C609977B49C}"/>
-    <hyperlink ref="F118" r:id="rId106" display="Kony@123" xr:uid="{52311FF1-9CF6-428D-B8C0-3A7E10D7A9D8}"/>
+    <hyperlink ref="F118" r:id="rId106" xr:uid="{52311FF1-9CF6-428D-B8C0-3A7E10D7A9D8}"/>
     <hyperlink ref="F119" r:id="rId107" display="Kony@123" xr:uid="{31B94F7C-1214-4F06-BF23-C50F49679A20}"/>
     <hyperlink ref="F120" r:id="rId108" display="Kony@123" xr:uid="{3BE685BC-E79E-4D92-B932-EAF4EACAC356}"/>
     <hyperlink ref="F121" r:id="rId109" display="Kony@123" xr:uid="{E32DB1B7-A3E9-4CE2-9B76-432AD9C6A165}"/>
@@ -4198,9 +4201,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4210,7 +4213,7 @@
     <col min="3" max="3" width="12" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="35" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.85546875" bestFit="1" customWidth="1"/>
@@ -4326,7 +4329,7 @@
         <v>268</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>21</v>
@@ -4416,7 +4419,7 @@
         <v>46</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>324</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modified scripts of Q2
</commit_message>
<xml_diff>
--- a/Q2_Automation/src/main/java/com/Resources/TestData.xlsx
+++ b/Q2_Automation/src/main/java/com/Resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v6_Project_updates\TDECUProjects\Q2_Automation\src\main\java\com\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0052FF7E-BC73-43A2-83E5-C89975016A49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088EC0F7-9969-4515-B529-65C50D0A80DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1299" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="328">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -178,9 +178,6 @@
     <t>C23408_VerifyRepeatForeverCheckBox</t>
   </si>
   <si>
-    <t>1st of the month</t>
-  </si>
-  <si>
     <t>Repeat Forever</t>
   </si>
   <si>
@@ -580,12 +577,6 @@
     <t>C23500_VerifyMakeMortageLoanPayment</t>
   </si>
   <si>
-    <t>927878595</t>
-  </si>
-  <si>
-    <t>2445058</t>
-  </si>
-  <si>
     <t>C23505_VerifyAlertEdit</t>
   </si>
   <si>
@@ -598,9 +589,6 @@
     <t>Kony@1234</t>
   </si>
   <si>
-    <t>-2445</t>
-  </si>
-  <si>
     <t>consumer loan</t>
   </si>
   <si>
@@ -682,9 +670,6 @@
     <t>C23642_VerifyActivityCenterTransactionDetails</t>
   </si>
   <si>
-    <t>70024450</t>
-  </si>
-  <si>
     <t>60</t>
   </si>
   <si>
@@ -763,9 +748,6 @@
     <t>C23669_VerifyActivityCenterTransactionFilteringWithTransactionID</t>
   </si>
   <si>
-    <t>8413626</t>
-  </si>
-  <si>
     <t>C23509_VerifyMoreInfoAboutCompany</t>
   </si>
   <si>
@@ -913,18 +895,6 @@
     <t>KEL</t>
   </si>
   <si>
-    <t>20159539</t>
-  </si>
-  <si>
-    <t>2015953066</t>
-  </si>
-  <si>
-    <t>-2015953</t>
-  </si>
-  <si>
-    <t>Test@123</t>
-  </si>
-  <si>
     <t>C24234_VerifyChangeMyAddressOptionUnderSettings</t>
   </si>
   <si>
@@ -1016,6 +986,45 @@
   </si>
   <si>
     <t>1st day of the month</t>
+  </si>
+  <si>
+    <t>16471628</t>
+  </si>
+  <si>
+    <t>20464178</t>
+  </si>
+  <si>
+    <t>GUE</t>
+  </si>
+  <si>
+    <t>2028749100</t>
+  </si>
+  <si>
+    <t>MIT</t>
+  </si>
+  <si>
+    <t>-42471</t>
+  </si>
+  <si>
+    <t>20333043</t>
+  </si>
+  <si>
+    <t>926055682</t>
+  </si>
+  <si>
+    <t>user2028749</t>
+  </si>
+  <si>
+    <t>2028749601</t>
+  </si>
+  <si>
+    <t>-12813</t>
+  </si>
+  <si>
+    <t>12813100</t>
+  </si>
+  <si>
+    <t>12813055</t>
   </si>
 </sst>
 </file>
@@ -1417,8 +1426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="80" workbookViewId="0">
-      <selection activeCell="F118" sqref="F118"/>
+    <sheetView topLeftCell="A71" zoomScale="80" workbookViewId="0">
+      <selection activeCell="E102" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,10 +1474,10 @@
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1485,10 +1494,10 @@
         <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1505,10 +1514,10 @@
         <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1525,10 +1534,10 @@
         <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1545,10 +1554,10 @@
         <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1565,15 +1574,15 @@
         <v>12</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>17</v>
@@ -1585,15 +1594,15 @@
         <v>12</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>17</v>
@@ -1605,10 +1614,10 @@
         <v>12</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1625,10 +1634,10 @@
         <v>12</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1645,15 +1654,15 @@
         <v>12</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>17</v>
@@ -1665,10 +1674,10 @@
         <v>12</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1685,10 +1694,10 @@
         <v>12</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1705,10 +1714,10 @@
         <v>12</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1725,10 +1734,10 @@
         <v>12</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1773,10 +1782,10 @@
         <v>12</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1793,10 +1802,10 @@
         <v>12</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1833,10 +1842,10 @@
         <v>12</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1853,10 +1862,10 @@
         <v>12</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1873,15 +1882,15 @@
         <v>12</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>17</v>
@@ -1893,15 +1902,15 @@
         <v>12</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>17</v>
@@ -1913,15 +1922,15 @@
         <v>12</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>17</v>
@@ -1933,15 +1942,15 @@
         <v>12</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>17</v>
@@ -1953,15 +1962,15 @@
         <v>12</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>17</v>
@@ -1973,15 +1982,15 @@
         <v>12</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>17</v>
@@ -1993,15 +2002,15 @@
         <v>12</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>17</v>
@@ -2013,15 +2022,15 @@
         <v>12</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>17</v>
@@ -2033,15 +2042,15 @@
         <v>12</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>17</v>
@@ -2053,15 +2062,15 @@
         <v>12</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>17</v>
@@ -2073,15 +2082,15 @@
         <v>12</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="B34" s="7" t="s">
         <v>17</v>
@@ -2093,7 +2102,7 @@
         <v>12</v>
       </c>
       <c r="E34" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>15</v>
@@ -2101,7 +2110,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="B35" s="7" t="s">
         <v>17</v>
@@ -2113,7 +2122,7 @@
         <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>15</v>
@@ -2121,7 +2130,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>17</v>
@@ -2133,7 +2142,7 @@
         <v>12</v>
       </c>
       <c r="E36" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>15</v>
@@ -2141,19 +2150,19 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>291</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" t="s">
         <v>301</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C37" t="s">
-        <v>10</v>
-      </c>
-      <c r="D37" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" t="s">
-        <v>311</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>15</v>
@@ -2161,7 +2170,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="B38" s="7" t="s">
         <v>17</v>
@@ -2173,7 +2182,7 @@
         <v>12</v>
       </c>
       <c r="E38" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>15</v>
@@ -2181,7 +2190,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="B39" s="7" t="s">
         <v>17</v>
@@ -2193,7 +2202,7 @@
         <v>12</v>
       </c>
       <c r="E39" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>15</v>
@@ -2201,7 +2210,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="B40" s="7" t="s">
         <v>17</v>
@@ -2213,7 +2222,7 @@
         <v>12</v>
       </c>
       <c r="E40" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>15</v>
@@ -2221,7 +2230,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="B41" s="7" t="s">
         <v>17</v>
@@ -2233,7 +2242,7 @@
         <v>12</v>
       </c>
       <c r="E41" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>15</v>
@@ -2241,7 +2250,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="B42" s="7" t="s">
         <v>17</v>
@@ -2253,7 +2262,7 @@
         <v>12</v>
       </c>
       <c r="E42" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>15</v>
@@ -2261,7 +2270,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>17</v>
@@ -2273,15 +2282,15 @@
         <v>12</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B44" s="7" t="s">
         <v>17</v>
@@ -2293,15 +2302,15 @@
         <v>12</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B45" s="7" t="s">
         <v>17</v>
@@ -2313,15 +2322,15 @@
         <v>12</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>17</v>
@@ -2333,15 +2342,15 @@
         <v>12</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>17</v>
@@ -2353,15 +2362,15 @@
         <v>12</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>17</v>
@@ -2373,15 +2382,15 @@
         <v>12</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>17</v>
@@ -2393,15 +2402,15 @@
         <v>12</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>17</v>
@@ -2413,15 +2422,15 @@
         <v>12</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>17</v>
@@ -2433,15 +2442,15 @@
         <v>12</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>17</v>
@@ -2453,15 +2462,15 @@
         <v>12</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>17</v>
@@ -2473,15 +2482,15 @@
         <v>12</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>17</v>
@@ -2493,15 +2502,15 @@
         <v>12</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>17</v>
@@ -2513,15 +2522,15 @@
         <v>12</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B56" s="7" t="s">
         <v>17</v>
@@ -2533,15 +2542,15 @@
         <v>12</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B57" s="7" t="s">
         <v>17</v>
@@ -2553,15 +2562,15 @@
         <v>12</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B58" s="7" t="s">
         <v>17</v>
@@ -2573,15 +2582,15 @@
         <v>12</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B59" s="7" t="s">
         <v>17</v>
@@ -2593,15 +2602,15 @@
         <v>12</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B60" s="7" t="s">
         <v>17</v>
@@ -2613,15 +2622,15 @@
         <v>12</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>17</v>
@@ -2633,15 +2642,15 @@
         <v>12</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>17</v>
@@ -2653,15 +2662,15 @@
         <v>12</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B63" s="7" t="s">
         <v>17</v>
@@ -2673,15 +2682,15 @@
         <v>12</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B64" s="7" t="s">
         <v>17</v>
@@ -2693,15 +2702,15 @@
         <v>12</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B65" s="7" t="s">
         <v>17</v>
@@ -2713,15 +2722,15 @@
         <v>12</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B66" s="7" t="s">
         <v>17</v>
@@ -2733,15 +2742,15 @@
         <v>12</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B67" s="7" t="s">
         <v>17</v>
@@ -2753,15 +2762,15 @@
         <v>12</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B68" s="7" t="s">
         <v>17</v>
@@ -2773,15 +2782,15 @@
         <v>12</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B69" s="7" t="s">
         <v>17</v>
@@ -2793,15 +2802,15 @@
         <v>12</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>17</v>
@@ -2813,15 +2822,15 @@
         <v>12</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>17</v>
@@ -2833,15 +2842,15 @@
         <v>12</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>17</v>
@@ -2853,15 +2862,15 @@
         <v>12</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>17</v>
@@ -2873,15 +2882,15 @@
         <v>12</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B74" s="7" t="s">
         <v>17</v>
@@ -2893,15 +2902,15 @@
         <v>12</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B75" s="7" t="s">
         <v>17</v>
@@ -2913,15 +2922,15 @@
         <v>12</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B76" s="7" t="s">
         <v>17</v>
@@ -2933,15 +2942,15 @@
         <v>12</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B77" s="7" t="s">
         <v>17</v>
@@ -2953,15 +2962,15 @@
         <v>12</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>17</v>
@@ -2973,15 +2982,15 @@
         <v>12</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B79" s="7" t="s">
         <v>17</v>
@@ -2993,15 +3002,15 @@
         <v>12</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B80" s="7" t="s">
         <v>17</v>
@@ -3013,15 +3022,15 @@
         <v>12</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B81" s="7" t="s">
         <v>17</v>
@@ -3033,15 +3042,15 @@
         <v>12</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B82" s="7" t="s">
         <v>17</v>
@@ -3053,15 +3062,15 @@
         <v>12</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>185</v>
+        <v>320</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>15</v>
+        <v>312</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B83" s="7" t="s">
         <v>17</v>
@@ -3073,15 +3082,15 @@
         <v>12</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>185</v>
+        <v>325</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>15</v>
+        <v>312</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B84" s="7" t="s">
         <v>17</v>
@@ -3093,15 +3102,15 @@
         <v>12</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B85" s="7" t="s">
         <v>17</v>
@@ -3113,15 +3122,15 @@
         <v>12</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B86" s="7" t="s">
         <v>17</v>
@@ -3133,15 +3142,15 @@
         <v>12</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B87" s="7" t="s">
         <v>17</v>
@@ -3153,15 +3162,15 @@
         <v>12</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>185</v>
+        <v>320</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>15</v>
+        <v>312</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B88" s="7" t="s">
         <v>17</v>
@@ -3173,15 +3182,15 @@
         <v>12</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>185</v>
+        <v>325</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>15</v>
+        <v>312</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B89" s="7" t="s">
         <v>17</v>
@@ -3193,15 +3202,15 @@
         <v>12</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B90" s="7" t="s">
         <v>17</v>
@@ -3213,15 +3222,15 @@
         <v>12</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B91" s="7" t="s">
         <v>17</v>
@@ -3233,15 +3242,15 @@
         <v>12</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B92" s="7" t="s">
         <v>17</v>
@@ -3253,15 +3262,15 @@
         <v>12</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B93" s="7" t="s">
         <v>17</v>
@@ -3273,15 +3282,15 @@
         <v>12</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>185</v>
+        <v>320</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>15</v>
+        <v>312</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B94" s="7" t="s">
         <v>17</v>
@@ -3293,15 +3302,15 @@
         <v>12</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>292</v>
+        <v>323</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>293</v>
+        <v>312</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B95" s="7" t="s">
         <v>17</v>
@@ -3313,15 +3322,15 @@
         <v>12</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>185</v>
+        <v>325</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>15</v>
+        <v>312</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B96" s="7" t="s">
         <v>17</v>
@@ -3333,15 +3342,15 @@
         <v>12</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B97" s="7" t="s">
         <v>17</v>
@@ -3353,15 +3362,15 @@
         <v>12</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B98" s="7" t="s">
         <v>17</v>
@@ -3373,15 +3382,15 @@
         <v>12</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B99" s="7" t="s">
         <v>17</v>
@@ -3393,15 +3402,15 @@
         <v>12</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B100" s="7" t="s">
         <v>17</v>
@@ -3413,15 +3422,15 @@
         <v>12</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B101" s="7" t="s">
         <v>17</v>
@@ -3433,15 +3442,15 @@
         <v>12</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>185</v>
+        <v>320</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>15</v>
+        <v>312</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B102" s="7" t="s">
         <v>17</v>
@@ -3453,15 +3462,15 @@
         <v>12</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>185</v>
+        <v>323</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>15</v>
+        <v>312</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B103" s="7" t="s">
         <v>17</v>
@@ -3473,15 +3482,15 @@
         <v>12</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>185</v>
+        <v>325</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>15</v>
+        <v>312</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B104" s="7" t="s">
         <v>17</v>
@@ -3493,15 +3502,15 @@
         <v>12</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>185</v>
+        <v>325</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>15</v>
+        <v>312</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B105" s="7" t="s">
         <v>17</v>
@@ -3513,15 +3522,15 @@
         <v>12</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>185</v>
+        <v>320</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>15</v>
+        <v>312</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B106" s="7" t="s">
         <v>17</v>
@@ -3533,15 +3542,15 @@
         <v>12</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>292</v>
+        <v>323</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>293</v>
+        <v>312</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B107" s="7" t="s">
         <v>17</v>
@@ -3553,15 +3562,15 @@
         <v>12</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B108" s="7" t="s">
         <v>17</v>
@@ -3573,15 +3582,15 @@
         <v>12</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B109" s="7" t="s">
         <v>17</v>
@@ -3593,15 +3602,15 @@
         <v>12</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B110" s="7" t="s">
         <v>17</v>
@@ -3613,15 +3622,15 @@
         <v>12</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="B111" s="7" t="s">
         <v>17</v>
@@ -3633,15 +3642,15 @@
         <v>12</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B112" s="7" t="s">
         <v>17</v>
@@ -3653,15 +3662,15 @@
         <v>12</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B113" s="7" t="s">
         <v>17</v>
@@ -3673,15 +3682,15 @@
         <v>12</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B114" s="7" t="s">
         <v>17</v>
@@ -3693,15 +3702,15 @@
         <v>12</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B115" s="7" t="s">
         <v>17</v>
@@ -3713,15 +3722,15 @@
         <v>12</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B116" s="7" t="s">
         <v>17</v>
@@ -3733,15 +3742,15 @@
         <v>12</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B117" s="7" t="s">
         <v>17</v>
@@ -3753,15 +3762,15 @@
         <v>12</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B118" s="7" t="s">
         <v>17</v>
@@ -3773,15 +3782,15 @@
         <v>12</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B119" s="7" t="s">
         <v>17</v>
@@ -3793,15 +3802,15 @@
         <v>12</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B120" s="7" t="s">
         <v>17</v>
@@ -3813,15 +3822,15 @@
         <v>12</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="B121" s="7" t="s">
         <v>17</v>
@@ -3833,15 +3842,15 @@
         <v>12</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B122" s="7" t="s">
         <v>17</v>
@@ -3853,15 +3862,15 @@
         <v>12</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B123" s="7" t="s">
         <v>17</v>
@@ -3873,15 +3882,15 @@
         <v>12</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B124" s="7" t="s">
         <v>17</v>
@@ -3893,15 +3902,15 @@
         <v>12</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B125" s="7" t="s">
         <v>17</v>
@@ -3913,15 +3922,15 @@
         <v>12</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B126" s="7" t="s">
         <v>17</v>
@@ -3933,15 +3942,15 @@
         <v>12</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B127" s="7" t="s">
         <v>17</v>
@@ -3953,15 +3962,15 @@
         <v>12</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B128" s="7" t="s">
         <v>17</v>
@@ -3973,15 +3982,15 @@
         <v>12</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B129" s="7" t="s">
         <v>17</v>
@@ -3993,15 +4002,15 @@
         <v>12</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="B130" s="7" t="s">
         <v>17</v>
@@ -4013,15 +4022,15 @@
         <v>12</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B131" s="7" t="s">
         <v>17</v>
@@ -4033,15 +4042,15 @@
         <v>12</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B132" s="7" t="s">
         <v>17</v>
@@ -4053,144 +4062,144 @@
         <v>12</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
     <hyperlink ref="F82" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="F94" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="F101" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="F106" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="F34" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="F35" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="F36" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="F37" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="F38" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="F39" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="F40" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="F41" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="F42" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="F2" r:id="rId15" display="Kony@123" xr:uid="{C8290296-74F1-47C4-B98A-4A9B0B69BDD6}"/>
-    <hyperlink ref="F3" r:id="rId16" display="Kony@123" xr:uid="{6985B5AA-B658-404F-B361-7C2A8AFEE179}"/>
-    <hyperlink ref="F4" r:id="rId17" display="Kony@123" xr:uid="{848A4FF3-1F9A-4975-8DC1-D68CAB635E07}"/>
-    <hyperlink ref="F5" r:id="rId18" display="Kony@123" xr:uid="{8B2A9D04-18F2-4FA0-8693-D70C03481F9D}"/>
-    <hyperlink ref="F6" r:id="rId19" display="Kony@123" xr:uid="{54197B00-336A-4660-B1DE-7ED27D90B5BF}"/>
-    <hyperlink ref="F7" r:id="rId20" display="Kony@123" xr:uid="{32261720-EACB-4B4E-8C75-E041A7F9D488}"/>
-    <hyperlink ref="F8" r:id="rId21" display="Kony@123" xr:uid="{7C51A3FC-D85B-49AC-A00A-F8D91B8EB9DC}"/>
-    <hyperlink ref="F9" r:id="rId22" display="Kony@123" xr:uid="{12A08FB1-DED1-4EC3-BECF-606C3E2778AF}"/>
-    <hyperlink ref="F10" r:id="rId23" display="Kony@123" xr:uid="{9BF11E09-87D7-49E4-88D0-6BA6B40BBDB2}"/>
-    <hyperlink ref="F11" r:id="rId24" display="Kony@123" xr:uid="{0B13BDA1-92A3-40B9-B600-C680436BCB46}"/>
-    <hyperlink ref="F12" r:id="rId25" display="Kony@123" xr:uid="{A4B2AA20-AE85-401E-A4AC-DA2C8B85C069}"/>
-    <hyperlink ref="F13" r:id="rId26" display="Kony@123" xr:uid="{E694F999-DB4A-4E16-877A-0197AA295A6A}"/>
-    <hyperlink ref="F14" r:id="rId27" display="Kony@123" xr:uid="{9BEF8D2A-97FD-4D7C-A4E5-98F01BF31502}"/>
-    <hyperlink ref="F15" r:id="rId28" display="Kony@123" xr:uid="{64F7CE5A-4CB1-4C67-9582-D17D5ED8E4FE}"/>
-    <hyperlink ref="F18" r:id="rId29" display="Kony@123" xr:uid="{72D49926-85B3-4C08-9510-37BFEB7B489B}"/>
-    <hyperlink ref="F19" r:id="rId30" display="Kony@123" xr:uid="{87866760-2DB7-4039-B9C4-E96B865E9395}"/>
-    <hyperlink ref="F21" r:id="rId31" display="Kony@123" xr:uid="{F0653554-2308-48C5-9404-CB9C6D8A6B0C}"/>
-    <hyperlink ref="F22" r:id="rId32" display="Kony@123" xr:uid="{DF2C3F7B-EB99-4939-B8C2-8139B4A0B6E5}"/>
-    <hyperlink ref="F23" r:id="rId33" display="Kony@123" xr:uid="{3C98B11D-26F3-4FF1-8696-87BC8FE432DE}"/>
-    <hyperlink ref="F24" r:id="rId34" display="Kony@123" xr:uid="{F50DD16B-F3EF-41E8-916F-71185B9FC64C}"/>
-    <hyperlink ref="F25" r:id="rId35" display="Kony@123" xr:uid="{B820EB0C-6373-4A55-ACDA-16C9426E2360}"/>
-    <hyperlink ref="F26" r:id="rId36" display="Kony@123" xr:uid="{7FE49DA8-FD83-4B46-BF77-2F18B4F36EF9}"/>
-    <hyperlink ref="F27" r:id="rId37" display="Kony@123" xr:uid="{63AD937C-79A8-4971-814E-42CAF285E6FD}"/>
-    <hyperlink ref="F28" r:id="rId38" display="Kony@123" xr:uid="{60968FFA-A588-4D1E-AC4F-954F10C56AF3}"/>
-    <hyperlink ref="F29" r:id="rId39" display="Kony@123" xr:uid="{B15B5200-1276-4AA8-89D7-43A9197D41AF}"/>
-    <hyperlink ref="F30" r:id="rId40" display="Kony@123" xr:uid="{57BBCCD0-13DB-43BB-B028-F36F8CC317CC}"/>
-    <hyperlink ref="F31" r:id="rId41" display="Kony@123" xr:uid="{23BC9856-CB23-48C2-B1FB-E36BFDF229CE}"/>
-    <hyperlink ref="F32" r:id="rId42" display="Kony@123" xr:uid="{1014470F-0051-4145-A480-6F738A91D1B0}"/>
-    <hyperlink ref="F33" r:id="rId43" display="Kony@123" xr:uid="{9563D07C-7B00-4285-A678-F0388C4AAC6C}"/>
-    <hyperlink ref="F43" r:id="rId44" display="Kony@123" xr:uid="{112CF6B3-0086-45DB-B506-305E30DD5F33}"/>
-    <hyperlink ref="F44" r:id="rId45" display="Kony@123" xr:uid="{A6FFE977-C3AC-449E-A3F1-35E8ECC18243}"/>
-    <hyperlink ref="F45" r:id="rId46" display="Kony@123" xr:uid="{20BFF49F-3D9E-4DA3-B0B4-3EDBB6DF93F1}"/>
-    <hyperlink ref="F46" r:id="rId47" display="Kony@123" xr:uid="{CD82CA82-782B-4594-AC15-19544D9F9C8B}"/>
-    <hyperlink ref="F47" r:id="rId48" display="Kony@123" xr:uid="{38A7D0DD-DE6E-4293-8E02-C74B6526F10B}"/>
-    <hyperlink ref="F48" r:id="rId49" display="Kony@123" xr:uid="{F21DF479-80D7-4875-A66D-72DA5E449D30}"/>
-    <hyperlink ref="F49" r:id="rId50" display="Kony@123" xr:uid="{C43106AF-CE48-4D4D-9F44-4B220B53DECE}"/>
-    <hyperlink ref="F50" r:id="rId51" display="Kony@123" xr:uid="{CA6EFCAE-911B-47E9-BF2E-DAA2209E7A71}"/>
-    <hyperlink ref="F51" r:id="rId52" display="Kony@123" xr:uid="{09570598-1CCC-470F-8A5E-6801A155BFF0}"/>
-    <hyperlink ref="F52" r:id="rId53" display="Kony@123" xr:uid="{38F26C89-EBE2-46F3-98BB-1A7378135234}"/>
-    <hyperlink ref="F53" r:id="rId54" display="Kony@123" xr:uid="{1686E96D-707F-4A18-ACA6-935646170B3D}"/>
-    <hyperlink ref="F54" r:id="rId55" display="Kony@123" xr:uid="{1619FB29-A79D-4E6B-B4A2-D956D14FAC45}"/>
-    <hyperlink ref="F55" r:id="rId56" display="Kony@123" xr:uid="{CE7CEF5D-E058-4C89-94D7-99A6CDE97CB3}"/>
-    <hyperlink ref="F56" r:id="rId57" display="Kony@123" xr:uid="{2EDE3577-F6A7-4F5B-AFB7-BC92AC6F59AF}"/>
-    <hyperlink ref="F57" r:id="rId58" display="Kony@123" xr:uid="{81F5DA1F-7FFF-4B4C-9928-6F3302B1E637}"/>
-    <hyperlink ref="F58" r:id="rId59" display="Kony@123" xr:uid="{73E4B230-6257-45E3-978D-06EBE2261946}"/>
-    <hyperlink ref="F59" r:id="rId60" display="Kony@123" xr:uid="{AC08AD28-BE28-49AD-B4D5-45164A26DEA5}"/>
-    <hyperlink ref="F60" r:id="rId61" display="Kony@123" xr:uid="{4AE8FEBB-3253-4FE4-AF78-DCC4AF8BD33C}"/>
-    <hyperlink ref="F61" r:id="rId62" display="Kony@123" xr:uid="{15218EE4-B510-40F6-B18B-2A01E2F3EC7E}"/>
-    <hyperlink ref="F62" r:id="rId63" display="Kony@123" xr:uid="{A249844A-EFD7-4C54-84B3-52CAB7B2E8E5}"/>
-    <hyperlink ref="F63" r:id="rId64" display="Kony@123" xr:uid="{1A963F5C-5948-4203-8AAD-2A5B688A7E3D}"/>
-    <hyperlink ref="F64" r:id="rId65" display="Kony@123" xr:uid="{72A376C6-204F-4076-9667-E94EB401CAA0}"/>
-    <hyperlink ref="F65" r:id="rId66" display="Kony@123" xr:uid="{3B0DFB31-690D-4922-BF6E-E1EA30C36A51}"/>
-    <hyperlink ref="F66" r:id="rId67" display="Kony@123" xr:uid="{57A0819C-2069-4906-BA64-16F8BA866D9D}"/>
-    <hyperlink ref="F67" r:id="rId68" display="Kony@123" xr:uid="{49690EA3-8504-4FDE-97F0-61DC470952BA}"/>
-    <hyperlink ref="F68" r:id="rId69" display="Kony@123" xr:uid="{EEBB06B6-9044-406C-A3A1-99B83FABCADC}"/>
-    <hyperlink ref="F69" r:id="rId70" display="Kony@123" xr:uid="{81B733E6-78EE-4E7B-8E2C-DF0B7107C340}"/>
-    <hyperlink ref="F70" r:id="rId71" display="Kony@123" xr:uid="{0082AC9D-7E42-43B9-9BC7-669DF312F639}"/>
-    <hyperlink ref="F71" r:id="rId72" display="Kony@123" xr:uid="{20E7F5E7-FD1D-4162-B621-BD95048B4766}"/>
-    <hyperlink ref="F72" r:id="rId73" display="Kony@123" xr:uid="{5C90467E-B95F-4FAF-9C90-0E68CC2FE2D3}"/>
-    <hyperlink ref="F73" r:id="rId74" display="Kony@123" xr:uid="{ABBCD72D-A485-4FD5-AE43-55DE7E771213}"/>
-    <hyperlink ref="F74" r:id="rId75" display="Kony@123" xr:uid="{154490DA-872A-4FF9-B2BE-E30515995EB3}"/>
-    <hyperlink ref="F75" r:id="rId76" display="Kony@123" xr:uid="{76BC609C-5D7E-4DE9-AFA9-B69B19DAF792}"/>
-    <hyperlink ref="F76" r:id="rId77" display="Kony@123" xr:uid="{45BB160F-B547-48E0-944F-E82BBD2014AA}"/>
-    <hyperlink ref="F77" r:id="rId78" display="Kony@123" xr:uid="{967ECF78-A7CE-47D3-8E74-BCBD8059EA58}"/>
-    <hyperlink ref="F78" r:id="rId79" display="Kony@123" xr:uid="{03E8D44D-7B7B-473C-972D-22B492AC0C27}"/>
-    <hyperlink ref="F79" r:id="rId80" display="Kony@123" xr:uid="{86026426-B2A1-4AD8-8DF6-D69A61A6E8AB}"/>
-    <hyperlink ref="F80" r:id="rId81" display="Kony@123" xr:uid="{923043A5-868E-48CC-88AA-37C72D4C492B}"/>
-    <hyperlink ref="F81" r:id="rId82" display="Kony@123" xr:uid="{5CD603BC-F856-4F58-AE54-2BA8049AC162}"/>
-    <hyperlink ref="F84" r:id="rId83" display="Kony@123" xr:uid="{514ECE2E-23FA-4E59-A8C9-D45D351CF8C4}"/>
-    <hyperlink ref="F85" r:id="rId84" display="Kony@123" xr:uid="{3E9898D1-01E9-4B42-A73F-FA5D49270409}"/>
-    <hyperlink ref="F86" r:id="rId85" display="Kony@123" xr:uid="{6C8A373E-4558-4549-B5CD-3092F837F805}"/>
-    <hyperlink ref="F89" r:id="rId86" display="Kony@123" xr:uid="{5368FA05-DE10-42A6-A357-B026967FDFC0}"/>
-    <hyperlink ref="F90" r:id="rId87" display="Kony@123" xr:uid="{E1573305-91A5-4A67-B827-21F0E01814D4}"/>
-    <hyperlink ref="F91" r:id="rId88" display="Kony@123" xr:uid="{EC5310D2-FE47-42C2-977E-73FDF3CEAC7F}"/>
-    <hyperlink ref="F92" r:id="rId89" display="Kony@123" xr:uid="{5C656A0E-C03F-46A5-9750-6448B7285932}"/>
-    <hyperlink ref="F96" r:id="rId90" display="Kony@123" xr:uid="{A98E7BB1-EEC6-456A-8058-3451A27FAC90}"/>
-    <hyperlink ref="F97" r:id="rId91" display="Kony@123" xr:uid="{E3228F97-3584-4DD5-ABD2-07E68F45C80C}"/>
-    <hyperlink ref="F98" r:id="rId92" display="Kony@123" xr:uid="{6DDF2FDE-838E-4322-8C71-F3918E530CF4}"/>
-    <hyperlink ref="F99" r:id="rId93" display="Kony@123" xr:uid="{D44CA776-25FA-44A0-95CB-A5EEF1FBF3C4}"/>
-    <hyperlink ref="F100" r:id="rId94" display="Kony@123" xr:uid="{B2523F64-9756-4607-B11E-1EB609E3938F}"/>
-    <hyperlink ref="F107" r:id="rId95" display="Kony@123" xr:uid="{1B50E80F-8635-4A37-A1B8-3EFE3126D967}"/>
-    <hyperlink ref="F108" r:id="rId96" display="Kony@123" xr:uid="{C59DFF30-5C77-41E6-AC81-0C18878AC7EA}"/>
-    <hyperlink ref="F109" r:id="rId97" display="Kony@123" xr:uid="{7A5D2A42-6072-4896-9F1E-31050D9437A9}"/>
-    <hyperlink ref="F110" r:id="rId98" display="Kony@123" xr:uid="{FA658073-1F5D-4D06-92E0-380D3101CCF6}"/>
-    <hyperlink ref="F111" r:id="rId99" display="Kony@123" xr:uid="{48C8A18E-E47D-4041-9989-7071F15DA0EC}"/>
-    <hyperlink ref="F112" r:id="rId100" display="Kony@123" xr:uid="{3A0583A7-FF13-45FD-9088-EFF63FFCBCD7}"/>
-    <hyperlink ref="F113" r:id="rId101" display="Kony@123" xr:uid="{21BDCC0D-E577-4717-9003-92D0D27274D4}"/>
-    <hyperlink ref="F114" r:id="rId102" display="Kony@123" xr:uid="{E7E2F38C-536F-473A-B8DD-5C8528E5FE37}"/>
-    <hyperlink ref="F115" r:id="rId103" display="Kony@123" xr:uid="{C2E080EC-EE6D-4EBC-B2BE-24781ADB0442}"/>
-    <hyperlink ref="F116" r:id="rId104" display="Kony@123" xr:uid="{3187464A-9470-4D02-9F1E-52C4C055ECF2}"/>
-    <hyperlink ref="F117" r:id="rId105" display="Kony@123" xr:uid="{159DA2BB-A519-4242-B0EA-1C609977B49C}"/>
-    <hyperlink ref="F118" r:id="rId106" xr:uid="{52311FF1-9CF6-428D-B8C0-3A7E10D7A9D8}"/>
-    <hyperlink ref="F119" r:id="rId107" display="Kony@123" xr:uid="{31B94F7C-1214-4F06-BF23-C50F49679A20}"/>
-    <hyperlink ref="F120" r:id="rId108" display="Kony@123" xr:uid="{3BE685BC-E79E-4D92-B932-EAF4EACAC356}"/>
-    <hyperlink ref="F121" r:id="rId109" display="Kony@123" xr:uid="{E32DB1B7-A3E9-4CE2-9B76-432AD9C6A165}"/>
-    <hyperlink ref="F122" r:id="rId110" display="Kony@123" xr:uid="{F4F85C7F-8CF5-4546-A8BE-4ABB56B6C27E}"/>
-    <hyperlink ref="F123" r:id="rId111" display="Kony@123" xr:uid="{17F58A17-F652-4FE7-A79C-4C582CE9E1EE}"/>
-    <hyperlink ref="F128" r:id="rId112" display="Kony@123" xr:uid="{170A913B-DD8E-42D1-BE29-4560950D3879}"/>
-    <hyperlink ref="F129" r:id="rId113" display="Kony@123" xr:uid="{F4B90F07-77BB-46A1-9696-53FA14BE033C}"/>
-    <hyperlink ref="F130" r:id="rId114" display="Kony@123" xr:uid="{782935E3-2C87-43AE-B37F-D81167DC6C56}"/>
-    <hyperlink ref="F131" r:id="rId115" display="Kony@123" xr:uid="{46EFFD81-5FAA-4270-91E5-E92AB19C13B8}"/>
-    <hyperlink ref="F132" r:id="rId116" display="Kony@123" xr:uid="{821C6BBE-7174-4880-86C5-57EB4864C07D}"/>
-    <hyperlink ref="F102" r:id="rId117" xr:uid="{4FC8F3C8-F05F-4087-87EE-11228151F75C}"/>
-    <hyperlink ref="F103" r:id="rId118" xr:uid="{EE6CA904-C919-419A-AD19-349869B95643}"/>
-    <hyperlink ref="F104" r:id="rId119" xr:uid="{A6980C23-F3B5-405B-88CA-DDED3E3953A6}"/>
-    <hyperlink ref="F105" r:id="rId120" xr:uid="{F16412BF-08B4-4A7C-9458-742ADBC51683}"/>
-    <hyperlink ref="F95" r:id="rId121" xr:uid="{2A36A62C-A1FC-4C05-8FCB-186013543287}"/>
-    <hyperlink ref="F93" r:id="rId122" xr:uid="{645750B4-482A-4D9B-B669-CED399B225D5}"/>
-    <hyperlink ref="F87" r:id="rId123" xr:uid="{A2400790-F78C-46C0-88D3-BDA7AD005E2D}"/>
-    <hyperlink ref="F88" r:id="rId124" xr:uid="{96BC7771-486E-4B34-99C1-D1BC03774B79}"/>
-    <hyperlink ref="F83" r:id="rId125" xr:uid="{992B7C17-9EFF-4783-BC97-23668AD262D0}"/>
-    <hyperlink ref="F124:F127" r:id="rId126" display="Kony@123" xr:uid="{609C902F-A8C4-4418-9AF6-A380CE4B9CB4}"/>
-    <hyperlink ref="F124" r:id="rId127" display="Kony@123" xr:uid="{5DBC08E0-01B2-417C-A59F-7C35CAF06534}"/>
-    <hyperlink ref="F125" r:id="rId128" display="Kony@123" xr:uid="{02499E77-EEE7-498B-AEC7-3709A2710756}"/>
-    <hyperlink ref="F126" r:id="rId129" display="Kony@123" xr:uid="{7D0F5AFC-3C66-49BE-A373-A74A3D84BA98}"/>
-    <hyperlink ref="F127" r:id="rId130" display="Kony@123" xr:uid="{2A8D54D2-DD8F-486C-9FF6-0A0567080352}"/>
+    <hyperlink ref="F34" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="F35" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="F36" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="F37" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="F38" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="F39" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="F40" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="F41" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="F42" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="F2" r:id="rId12" display="Kony@123" xr:uid="{C8290296-74F1-47C4-B98A-4A9B0B69BDD6}"/>
+    <hyperlink ref="F3" r:id="rId13" display="Kony@123" xr:uid="{6985B5AA-B658-404F-B361-7C2A8AFEE179}"/>
+    <hyperlink ref="F4" r:id="rId14" display="Kony@123" xr:uid="{848A4FF3-1F9A-4975-8DC1-D68CAB635E07}"/>
+    <hyperlink ref="F5" r:id="rId15" display="Kony@123" xr:uid="{8B2A9D04-18F2-4FA0-8693-D70C03481F9D}"/>
+    <hyperlink ref="F6" r:id="rId16" display="Kony@123" xr:uid="{54197B00-336A-4660-B1DE-7ED27D90B5BF}"/>
+    <hyperlink ref="F7" r:id="rId17" display="Kony@123" xr:uid="{32261720-EACB-4B4E-8C75-E041A7F9D488}"/>
+    <hyperlink ref="F8" r:id="rId18" display="Kony@123" xr:uid="{7C51A3FC-D85B-49AC-A00A-F8D91B8EB9DC}"/>
+    <hyperlink ref="F9" r:id="rId19" display="Kony@123" xr:uid="{12A08FB1-DED1-4EC3-BECF-606C3E2778AF}"/>
+    <hyperlink ref="F10" r:id="rId20" display="Kony@123" xr:uid="{9BF11E09-87D7-49E4-88D0-6BA6B40BBDB2}"/>
+    <hyperlink ref="F11" r:id="rId21" display="Kony@123" xr:uid="{0B13BDA1-92A3-40B9-B600-C680436BCB46}"/>
+    <hyperlink ref="F12" r:id="rId22" display="Kony@123" xr:uid="{A4B2AA20-AE85-401E-A4AC-DA2C8B85C069}"/>
+    <hyperlink ref="F13" r:id="rId23" display="Kony@123" xr:uid="{E694F999-DB4A-4E16-877A-0197AA295A6A}"/>
+    <hyperlink ref="F14" r:id="rId24" display="Kony@123" xr:uid="{9BEF8D2A-97FD-4D7C-A4E5-98F01BF31502}"/>
+    <hyperlink ref="F15" r:id="rId25" display="Kony@123" xr:uid="{64F7CE5A-4CB1-4C67-9582-D17D5ED8E4FE}"/>
+    <hyperlink ref="F18" r:id="rId26" display="Kony@123" xr:uid="{72D49926-85B3-4C08-9510-37BFEB7B489B}"/>
+    <hyperlink ref="F19" r:id="rId27" display="Kony@123" xr:uid="{87866760-2DB7-4039-B9C4-E96B865E9395}"/>
+    <hyperlink ref="F21" r:id="rId28" display="Kony@123" xr:uid="{F0653554-2308-48C5-9404-CB9C6D8A6B0C}"/>
+    <hyperlink ref="F22" r:id="rId29" display="Kony@123" xr:uid="{DF2C3F7B-EB99-4939-B8C2-8139B4A0B6E5}"/>
+    <hyperlink ref="F23" r:id="rId30" display="Kony@123" xr:uid="{3C98B11D-26F3-4FF1-8696-87BC8FE432DE}"/>
+    <hyperlink ref="F24" r:id="rId31" display="Kony@123" xr:uid="{F50DD16B-F3EF-41E8-916F-71185B9FC64C}"/>
+    <hyperlink ref="F25" r:id="rId32" display="Kony@123" xr:uid="{B820EB0C-6373-4A55-ACDA-16C9426E2360}"/>
+    <hyperlink ref="F26" r:id="rId33" display="Kony@123" xr:uid="{7FE49DA8-FD83-4B46-BF77-2F18B4F36EF9}"/>
+    <hyperlink ref="F27" r:id="rId34" display="Kony@123" xr:uid="{63AD937C-79A8-4971-814E-42CAF285E6FD}"/>
+    <hyperlink ref="F28" r:id="rId35" display="Kony@123" xr:uid="{60968FFA-A588-4D1E-AC4F-954F10C56AF3}"/>
+    <hyperlink ref="F29" r:id="rId36" display="Kony@123" xr:uid="{B15B5200-1276-4AA8-89D7-43A9197D41AF}"/>
+    <hyperlink ref="F30" r:id="rId37" display="Kony@123" xr:uid="{57BBCCD0-13DB-43BB-B028-F36F8CC317CC}"/>
+    <hyperlink ref="F31" r:id="rId38" display="Kony@123" xr:uid="{23BC9856-CB23-48C2-B1FB-E36BFDF229CE}"/>
+    <hyperlink ref="F32" r:id="rId39" display="Kony@123" xr:uid="{1014470F-0051-4145-A480-6F738A91D1B0}"/>
+    <hyperlink ref="F33" r:id="rId40" display="Kony@123" xr:uid="{9563D07C-7B00-4285-A678-F0388C4AAC6C}"/>
+    <hyperlink ref="F43" r:id="rId41" display="Kony@123" xr:uid="{112CF6B3-0086-45DB-B506-305E30DD5F33}"/>
+    <hyperlink ref="F44" r:id="rId42" display="Kony@123" xr:uid="{A6FFE977-C3AC-449E-A3F1-35E8ECC18243}"/>
+    <hyperlink ref="F45" r:id="rId43" display="Kony@123" xr:uid="{20BFF49F-3D9E-4DA3-B0B4-3EDBB6DF93F1}"/>
+    <hyperlink ref="F46" r:id="rId44" display="Kony@123" xr:uid="{CD82CA82-782B-4594-AC15-19544D9F9C8B}"/>
+    <hyperlink ref="F47" r:id="rId45" display="Kony@123" xr:uid="{38A7D0DD-DE6E-4293-8E02-C74B6526F10B}"/>
+    <hyperlink ref="F48" r:id="rId46" display="Kony@123" xr:uid="{F21DF479-80D7-4875-A66D-72DA5E449D30}"/>
+    <hyperlink ref="F49" r:id="rId47" display="Kony@123" xr:uid="{C43106AF-CE48-4D4D-9F44-4B220B53DECE}"/>
+    <hyperlink ref="F50" r:id="rId48" display="Kony@123" xr:uid="{CA6EFCAE-911B-47E9-BF2E-DAA2209E7A71}"/>
+    <hyperlink ref="F51" r:id="rId49" display="Kony@123" xr:uid="{09570598-1CCC-470F-8A5E-6801A155BFF0}"/>
+    <hyperlink ref="F52" r:id="rId50" display="Kony@123" xr:uid="{38F26C89-EBE2-46F3-98BB-1A7378135234}"/>
+    <hyperlink ref="F53" r:id="rId51" display="Kony@123" xr:uid="{1686E96D-707F-4A18-ACA6-935646170B3D}"/>
+    <hyperlink ref="F54" r:id="rId52" display="Kony@123" xr:uid="{1619FB29-A79D-4E6B-B4A2-D956D14FAC45}"/>
+    <hyperlink ref="F55" r:id="rId53" display="Kony@123" xr:uid="{CE7CEF5D-E058-4C89-94D7-99A6CDE97CB3}"/>
+    <hyperlink ref="F56" r:id="rId54" display="Kony@123" xr:uid="{2EDE3577-F6A7-4F5B-AFB7-BC92AC6F59AF}"/>
+    <hyperlink ref="F57" r:id="rId55" display="Kony@123" xr:uid="{81F5DA1F-7FFF-4B4C-9928-6F3302B1E637}"/>
+    <hyperlink ref="F58" r:id="rId56" display="Kony@123" xr:uid="{73E4B230-6257-45E3-978D-06EBE2261946}"/>
+    <hyperlink ref="F59" r:id="rId57" display="Kony@123" xr:uid="{AC08AD28-BE28-49AD-B4D5-45164A26DEA5}"/>
+    <hyperlink ref="F60" r:id="rId58" display="Kony@123" xr:uid="{4AE8FEBB-3253-4FE4-AF78-DCC4AF8BD33C}"/>
+    <hyperlink ref="F61" r:id="rId59" display="Kony@123" xr:uid="{15218EE4-B510-40F6-B18B-2A01E2F3EC7E}"/>
+    <hyperlink ref="F62" r:id="rId60" display="Kony@123" xr:uid="{A249844A-EFD7-4C54-84B3-52CAB7B2E8E5}"/>
+    <hyperlink ref="F63" r:id="rId61" display="Kony@123" xr:uid="{1A963F5C-5948-4203-8AAD-2A5B688A7E3D}"/>
+    <hyperlink ref="F64" r:id="rId62" display="Kony@123" xr:uid="{72A376C6-204F-4076-9667-E94EB401CAA0}"/>
+    <hyperlink ref="F65" r:id="rId63" display="Kony@123" xr:uid="{3B0DFB31-690D-4922-BF6E-E1EA30C36A51}"/>
+    <hyperlink ref="F66" r:id="rId64" display="Kony@123" xr:uid="{57A0819C-2069-4906-BA64-16F8BA866D9D}"/>
+    <hyperlink ref="F67" r:id="rId65" display="Kony@123" xr:uid="{49690EA3-8504-4FDE-97F0-61DC470952BA}"/>
+    <hyperlink ref="F68" r:id="rId66" display="Kony@123" xr:uid="{EEBB06B6-9044-406C-A3A1-99B83FABCADC}"/>
+    <hyperlink ref="F69" r:id="rId67" display="Kony@123" xr:uid="{81B733E6-78EE-4E7B-8E2C-DF0B7107C340}"/>
+    <hyperlink ref="F70" r:id="rId68" display="Kony@123" xr:uid="{0082AC9D-7E42-43B9-9BC7-669DF312F639}"/>
+    <hyperlink ref="F71" r:id="rId69" display="Kony@123" xr:uid="{20E7F5E7-FD1D-4162-B621-BD95048B4766}"/>
+    <hyperlink ref="F72" r:id="rId70" display="Kony@123" xr:uid="{5C90467E-B95F-4FAF-9C90-0E68CC2FE2D3}"/>
+    <hyperlink ref="F73" r:id="rId71" display="Kony@123" xr:uid="{ABBCD72D-A485-4FD5-AE43-55DE7E771213}"/>
+    <hyperlink ref="F74" r:id="rId72" display="Kony@123" xr:uid="{154490DA-872A-4FF9-B2BE-E30515995EB3}"/>
+    <hyperlink ref="F75" r:id="rId73" display="Kony@123" xr:uid="{76BC609C-5D7E-4DE9-AFA9-B69B19DAF792}"/>
+    <hyperlink ref="F76" r:id="rId74" display="Kony@123" xr:uid="{45BB160F-B547-48E0-944F-E82BBD2014AA}"/>
+    <hyperlink ref="F77" r:id="rId75" display="Kony@123" xr:uid="{967ECF78-A7CE-47D3-8E74-BCBD8059EA58}"/>
+    <hyperlink ref="F78" r:id="rId76" display="Kony@123" xr:uid="{03E8D44D-7B7B-473C-972D-22B492AC0C27}"/>
+    <hyperlink ref="F79" r:id="rId77" display="Kony@123" xr:uid="{86026426-B2A1-4AD8-8DF6-D69A61A6E8AB}"/>
+    <hyperlink ref="F80" r:id="rId78" display="Kony@123" xr:uid="{923043A5-868E-48CC-88AA-37C72D4C492B}"/>
+    <hyperlink ref="F81" r:id="rId79" display="Kony@123" xr:uid="{5CD603BC-F856-4F58-AE54-2BA8049AC162}"/>
+    <hyperlink ref="F84" r:id="rId80" display="Kony@123" xr:uid="{514ECE2E-23FA-4E59-A8C9-D45D351CF8C4}"/>
+    <hyperlink ref="F85" r:id="rId81" display="Kony@123" xr:uid="{3E9898D1-01E9-4B42-A73F-FA5D49270409}"/>
+    <hyperlink ref="F86" r:id="rId82" display="Kony@123" xr:uid="{6C8A373E-4558-4549-B5CD-3092F837F805}"/>
+    <hyperlink ref="F89" r:id="rId83" display="Kony@123" xr:uid="{5368FA05-DE10-42A6-A357-B026967FDFC0}"/>
+    <hyperlink ref="F90" r:id="rId84" display="Kony@123" xr:uid="{E1573305-91A5-4A67-B827-21F0E01814D4}"/>
+    <hyperlink ref="F91" r:id="rId85" display="Kony@123" xr:uid="{EC5310D2-FE47-42C2-977E-73FDF3CEAC7F}"/>
+    <hyperlink ref="F92" r:id="rId86" display="Kony@123" xr:uid="{5C656A0E-C03F-46A5-9750-6448B7285932}"/>
+    <hyperlink ref="F96" r:id="rId87" display="Kony@123" xr:uid="{A98E7BB1-EEC6-456A-8058-3451A27FAC90}"/>
+    <hyperlink ref="F97" r:id="rId88" display="Kony@123" xr:uid="{E3228F97-3584-4DD5-ABD2-07E68F45C80C}"/>
+    <hyperlink ref="F98" r:id="rId89" display="Kony@123" xr:uid="{6DDF2FDE-838E-4322-8C71-F3918E530CF4}"/>
+    <hyperlink ref="F99" r:id="rId90" display="Kony@123" xr:uid="{D44CA776-25FA-44A0-95CB-A5EEF1FBF3C4}"/>
+    <hyperlink ref="F100" r:id="rId91" display="Kony@123" xr:uid="{B2523F64-9756-4607-B11E-1EB609E3938F}"/>
+    <hyperlink ref="F107" r:id="rId92" display="Kony@123" xr:uid="{1B50E80F-8635-4A37-A1B8-3EFE3126D967}"/>
+    <hyperlink ref="F108" r:id="rId93" display="Kony@123" xr:uid="{C59DFF30-5C77-41E6-AC81-0C18878AC7EA}"/>
+    <hyperlink ref="F109" r:id="rId94" display="Kony@123" xr:uid="{7A5D2A42-6072-4896-9F1E-31050D9437A9}"/>
+    <hyperlink ref="F110" r:id="rId95" display="Kony@123" xr:uid="{FA658073-1F5D-4D06-92E0-380D3101CCF6}"/>
+    <hyperlink ref="F111" r:id="rId96" display="Kony@123" xr:uid="{48C8A18E-E47D-4041-9989-7071F15DA0EC}"/>
+    <hyperlink ref="F112" r:id="rId97" display="Kony@123" xr:uid="{3A0583A7-FF13-45FD-9088-EFF63FFCBCD7}"/>
+    <hyperlink ref="F113" r:id="rId98" display="Kony@123" xr:uid="{21BDCC0D-E577-4717-9003-92D0D27274D4}"/>
+    <hyperlink ref="F114" r:id="rId99" display="Kony@123" xr:uid="{E7E2F38C-536F-473A-B8DD-5C8528E5FE37}"/>
+    <hyperlink ref="F115" r:id="rId100" display="Kony@123" xr:uid="{C2E080EC-EE6D-4EBC-B2BE-24781ADB0442}"/>
+    <hyperlink ref="F116" r:id="rId101" display="Kony@123" xr:uid="{3187464A-9470-4D02-9F1E-52C4C055ECF2}"/>
+    <hyperlink ref="F117" r:id="rId102" display="Kony@123" xr:uid="{159DA2BB-A519-4242-B0EA-1C609977B49C}"/>
+    <hyperlink ref="F118" r:id="rId103" xr:uid="{52311FF1-9CF6-428D-B8C0-3A7E10D7A9D8}"/>
+    <hyperlink ref="F119" r:id="rId104" display="Kony@123" xr:uid="{31B94F7C-1214-4F06-BF23-C50F49679A20}"/>
+    <hyperlink ref="F120" r:id="rId105" display="Kony@123" xr:uid="{3BE685BC-E79E-4D92-B932-EAF4EACAC356}"/>
+    <hyperlink ref="F121" r:id="rId106" display="Kony@123" xr:uid="{E32DB1B7-A3E9-4CE2-9B76-432AD9C6A165}"/>
+    <hyperlink ref="F122" r:id="rId107" display="Kony@123" xr:uid="{F4F85C7F-8CF5-4546-A8BE-4ABB56B6C27E}"/>
+    <hyperlink ref="F123" r:id="rId108" display="Kony@123" xr:uid="{17F58A17-F652-4FE7-A79C-4C582CE9E1EE}"/>
+    <hyperlink ref="F128" r:id="rId109" display="Kony@123" xr:uid="{170A913B-DD8E-42D1-BE29-4560950D3879}"/>
+    <hyperlink ref="F129" r:id="rId110" display="Kony@123" xr:uid="{F4B90F07-77BB-46A1-9696-53FA14BE033C}"/>
+    <hyperlink ref="F130" r:id="rId111" display="Kony@123" xr:uid="{782935E3-2C87-43AE-B37F-D81167DC6C56}"/>
+    <hyperlink ref="F131" r:id="rId112" display="Kony@123" xr:uid="{46EFFD81-5FAA-4270-91E5-E92AB19C13B8}"/>
+    <hyperlink ref="F132" r:id="rId113" display="Kony@123" xr:uid="{821C6BBE-7174-4880-86C5-57EB4864C07D}"/>
+    <hyperlink ref="F124:F127" r:id="rId114" display="Kony@123" xr:uid="{609C902F-A8C4-4418-9AF6-A380CE4B9CB4}"/>
+    <hyperlink ref="F124" r:id="rId115" display="Kony@123" xr:uid="{5DBC08E0-01B2-417C-A59F-7C35CAF06534}"/>
+    <hyperlink ref="F125" r:id="rId116" display="Kony@123" xr:uid="{02499E77-EEE7-498B-AEC7-3709A2710756}"/>
+    <hyperlink ref="F126" r:id="rId117" display="Kony@123" xr:uid="{7D0F5AFC-3C66-49BE-A373-A74A3D84BA98}"/>
+    <hyperlink ref="F127" r:id="rId118" display="Kony@123" xr:uid="{2A8D54D2-DD8F-486C-9FF6-0A0567080352}"/>
+    <hyperlink ref="F93" r:id="rId119" xr:uid="{E79FD8E2-0811-4DD3-B83F-C8B1A04675C0}"/>
+    <hyperlink ref="F101" r:id="rId120" display="Kony@123" xr:uid="{E75E4D25-F5E1-4A39-8AF4-F5C3C34DF9D1}"/>
+    <hyperlink ref="F105" r:id="rId121" display="Kony@123" xr:uid="{5B762541-6788-4ECE-AE0A-1083A12FCA23}"/>
+    <hyperlink ref="F87" r:id="rId122" display="Kony@123" xr:uid="{62C1012E-874C-485C-A458-1A50D85C315E}"/>
+    <hyperlink ref="F106" r:id="rId123" display="Kony@123" xr:uid="{12217BC4-A8EF-4F82-872A-849862FE2F7B}"/>
+    <hyperlink ref="F94" r:id="rId124" display="Kony@123" xr:uid="{9673AC35-19D2-49B2-861E-4616721D221B}"/>
+    <hyperlink ref="F102" r:id="rId125" xr:uid="{0D14B215-7B6A-48D2-A6A1-3286340DEFDF}"/>
+    <hyperlink ref="F83" r:id="rId126" xr:uid="{B05A5C93-B446-44C8-9210-79F00F77CA67}"/>
+    <hyperlink ref="F88" r:id="rId127" xr:uid="{DBADFF1E-7913-4900-BF8C-A2457EF00E6E}"/>
+    <hyperlink ref="F95" r:id="rId128" xr:uid="{E8CB30C7-EED5-475A-AA4C-3BBA59D579F2}"/>
+    <hyperlink ref="F103" r:id="rId129" xr:uid="{0225E1B7-1DBD-4713-AFA3-9F849D4E1AC1}"/>
+    <hyperlink ref="F104" r:id="rId130" xr:uid="{98DE6044-3C3A-4B66-AF3A-A0BF803D4E97}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId131"/>
@@ -4199,11 +4208,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4246,25 +4255,25 @@
         <v>34</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="J1" s="3" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -4313,20 +4322,20 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>30</v>
@@ -4336,12 +4345,12 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>30</v>
@@ -4351,7 +4360,7 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -4369,7 +4378,7 @@
         <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -4383,7 +4392,7 @@
         <v>21</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E9" t="s">
         <v>38</v>
@@ -4416,15 +4425,15 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G11" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>30</v>
@@ -4433,18 +4442,18 @@
         <v>21</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>314</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>30</v>
@@ -4454,15 +4463,15 @@
       </c>
       <c r="D13" s="2"/>
       <c r="E13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" t="s">
         <v>57</v>
-      </c>
-      <c r="G13" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>20</v>
@@ -4471,12 +4480,12 @@
         <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>21</v>
@@ -4484,411 +4493,419 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H17" t="s">
+        <v>106</v>
+      </c>
+      <c r="I17" t="s">
         <v>107</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>108</v>
-      </c>
-      <c r="J17" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>213</v>
+        <v>321</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>179</v>
+        <v>322</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E18" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>213</v>
+        <v>326</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>180</v>
+        <v>327</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E19" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>213</v>
+        <v>321</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>179</v>
+        <v>322</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E22" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="G22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>213</v>
+        <v>326</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>180</v>
+        <v>327</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E23" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="G23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>213</v>
+        <v>321</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>179</v>
+        <v>322</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E24" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="G24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>290</v>
+        <v>318</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>291</v>
+        <v>324</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E25" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="G25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>213</v>
+        <v>326</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>180</v>
+        <v>327</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E26" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>213</v>
+        <v>321</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>179</v>
+        <v>322</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E27" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>213</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>223</v>
-      </c>
       <c r="E28" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>213</v>
+        <v>326</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>180</v>
+        <v>327</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E29" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>213</v>
+        <v>326</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>180</v>
+        <v>327</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E30" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>213</v>
+        <v>321</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>179</v>
+        <v>322</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E31" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>290</v>
+        <v>318</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>291</v>
+        <v>324</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E32" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="G32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>240</v>
+        <v>315</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>295</v>
-      </c>
-      <c r="J34" t="s">
-        <v>312</v>
-      </c>
-      <c r="L34" t="s">
-        <v>313</v>
-      </c>
-      <c r="M34" s="2" t="s">
-        <v>314</v>
+        <v>251</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="J35" t="s">
-        <v>312</v>
-      </c>
-      <c r="K35" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="L35" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="J36" t="s">
-        <v>312</v>
+        <v>302</v>
+      </c>
+      <c r="K36" t="s">
+        <v>305</v>
       </c>
       <c r="L36" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>291</v>
+      </c>
+      <c r="J37" t="s">
         <v>302</v>
       </c>
-      <c r="J37" t="s">
-        <v>318</v>
-      </c>
       <c r="L37" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="N37" s="8" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>292</v>
+      </c>
+      <c r="J38" t="s">
+        <v>308</v>
+      </c>
+      <c r="L38" t="s">
+        <v>306</v>
+      </c>
+      <c r="M38" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="L38" t="s">
-        <v>316</v>
-      </c>
-      <c r="M38" s="2" t="s">
-        <v>314</v>
+      <c r="N38" s="8" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>305</v>
-      </c>
-      <c r="J39" t="s">
-        <v>318</v>
-      </c>
-      <c r="K39" s="9" t="s">
-        <v>319</v>
+        <v>294</v>
       </c>
       <c r="L39" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="N39" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>295</v>
+      </c>
+      <c r="J40" t="s">
         <v>308</v>
       </c>
-      <c r="J40" t="s">
-        <v>318</v>
-      </c>
       <c r="K40" s="9" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="L40" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="N40" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>298</v>
+      </c>
+      <c r="J41" t="s">
+        <v>308</v>
+      </c>
+      <c r="K41" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="J41" t="s">
-        <v>318</v>
-      </c>
-      <c r="K41" s="9" t="s">
-        <v>319</v>
-      </c>
       <c r="L41" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="N41" t="s">
-        <v>310</v>
+        <v>297</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>299</v>
+      </c>
+      <c r="J42" t="s">
+        <v>308</v>
+      </c>
+      <c r="K42" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="L42" t="s">
+        <v>306</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="N42" t="s">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -4902,13 +4919,13 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B8"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -4921,180 +4938,180 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
         <v>51</v>
       </c>
-      <c r="D2" t="s">
-        <v>52</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>283</v>
+        <v>319</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>284</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D4" t="s">
-        <v>283</v>
+        <v>317</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>98</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D7" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D8" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -5112,7 +5129,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H115" r:id="rId1" display="Kony@789" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="H5" r:id="rId2" display="Kony@123" xr:uid="{FAFC8C47-05E1-4C5E-8F41-BE8F346CAB9A}"/>
+    <hyperlink ref="H5" r:id="rId2" xr:uid="{FAFC8C47-05E1-4C5E-8F41-BE8F346CAB9A}"/>
     <hyperlink ref="H6" r:id="rId3" display="Kony@123" xr:uid="{9EE8056A-AEBC-48DC-B153-AFBF5EFC0A39}"/>
     <hyperlink ref="H7" r:id="rId4" display="Kony@123" xr:uid="{EBA55935-094D-45EA-8CD4-0720D5439F75}"/>
     <hyperlink ref="H8" r:id="rId5" display="Kony@123" xr:uid="{3EF8C29D-D7F8-4190-AAAE-C947DD1C2DF4}"/>
@@ -5144,58 +5161,58 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
         <v>65</v>
       </c>
-      <c r="B2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -5209,7 +5226,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="H8" sqref="H8:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5231,112 +5248,118 @@
         <v>14</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" t="s">
         <v>74</v>
-      </c>
-      <c r="D2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E4" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D7" s="2"/>
       <c r="F7" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>228</v>
+        <v>223</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C9" s="2"/>
     </row>
@@ -5369,8 +5392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5393,154 +5416,154 @@
         <v>14</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>92</v>
-      </c>
       <c r="I1" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" t="s">
         <v>93</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" s="2"/>
       <c r="I3" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I4" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="J4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="D6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" t="s">
         <v>93</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="K6" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="I7" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="D8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F8" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" t="s">
         <v>93</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="L8" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -5571,118 +5594,118 @@
         <v>14</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F9" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
   </sheetData>
@@ -5715,286 +5738,286 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>154</v>
-      </c>
       <c r="K1" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" t="s">
         <v>122</v>
       </c>
-      <c r="B3" t="s">
-        <v>123</v>
-      </c>
       <c r="C3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" t="s">
         <v>128</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>129</v>
       </c>
-      <c r="F3" t="s">
-        <v>130</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E4" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E5" t="s">
         <v>136</v>
       </c>
-      <c r="B5" t="s">
-        <v>123</v>
-      </c>
-      <c r="C5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D5" t="s">
-        <v>128</v>
-      </c>
-      <c r="E5" t="s">
-        <v>137</v>
-      </c>
       <c r="F5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B6" t="s">
         <v>151</v>
       </c>
-      <c r="B6" t="s">
-        <v>152</v>
-      </c>
       <c r="D6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="J6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="J7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F8" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="J8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" t="s">
         <v>165</v>
       </c>
-      <c r="B9" t="s">
-        <v>166</v>
-      </c>
       <c r="D9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="2" t="s">
         <v>21</v>
       </c>
       <c r="J9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="2" t="s">
         <v>21</v>
       </c>
       <c r="J10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="2" t="s">
@@ -6004,129 +6027,129 @@
         <v>7</v>
       </c>
       <c r="K11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B12" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C12" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>21</v>
       </c>
       <c r="M12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B13" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C13" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>30</v>
       </c>
       <c r="M13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C14" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D14" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E15" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G15" s="2"/>
       <c r="I15" s="2" t="s">
         <v>21</v>
       </c>
       <c r="J15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E16" t="s">
+        <v>132</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -6165,7 +6188,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>15</v>
@@ -6176,10 +6199,10 @@
         <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Two tests added in test data sheet and locators too
</commit_message>
<xml_diff>
--- a/Q2_Automation/src/main/java/com/Resources/TestData.xlsx
+++ b/Q2_Automation/src/main/java/com/Resources/TestData.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v6_Project_updates\TDECUProjects\Q2_Automation\src\main\java\com\Resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088EC0F7-9969-4515-B529-65C50D0A80DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -23,7 +17,7 @@
     <sheet name="Alerts" sheetId="8" r:id="rId8"/>
     <sheet name="Login" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1305" uniqueCount="330">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1025,12 +1019,18 @@
   </si>
   <si>
     <t>12813055</t>
+  </si>
+  <si>
+    <t>C25165_VerifyAggregateExternalAccountfromLinkAccount</t>
+  </si>
+  <si>
+    <t>C25166_VerifyAggregateExternalAccountfromLinkAccountWidgetPage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1170,7 +1170,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1222,7 +1222,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1416,18 +1416,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F132"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" zoomScale="80" workbookViewId="0">
-      <selection activeCell="E102" sqref="E102"/>
+    <sheetView tabSelected="1" topLeftCell="A128" zoomScale="80" workbookViewId="0">
+      <selection activeCell="B134" sqref="B134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4068,138 +4068,148 @@
         <v>312</v>
       </c>
     </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>329</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="F82" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="F34" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="F35" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="F36" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="F37" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="F38" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="F39" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="F40" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="F41" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="F42" r:id="rId11" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="F2" r:id="rId12" display="Kony@123" xr:uid="{C8290296-74F1-47C4-B98A-4A9B0B69BDD6}"/>
-    <hyperlink ref="F3" r:id="rId13" display="Kony@123" xr:uid="{6985B5AA-B658-404F-B361-7C2A8AFEE179}"/>
-    <hyperlink ref="F4" r:id="rId14" display="Kony@123" xr:uid="{848A4FF3-1F9A-4975-8DC1-D68CAB635E07}"/>
-    <hyperlink ref="F5" r:id="rId15" display="Kony@123" xr:uid="{8B2A9D04-18F2-4FA0-8693-D70C03481F9D}"/>
-    <hyperlink ref="F6" r:id="rId16" display="Kony@123" xr:uid="{54197B00-336A-4660-B1DE-7ED27D90B5BF}"/>
-    <hyperlink ref="F7" r:id="rId17" display="Kony@123" xr:uid="{32261720-EACB-4B4E-8C75-E041A7F9D488}"/>
-    <hyperlink ref="F8" r:id="rId18" display="Kony@123" xr:uid="{7C51A3FC-D85B-49AC-A00A-F8D91B8EB9DC}"/>
-    <hyperlink ref="F9" r:id="rId19" display="Kony@123" xr:uid="{12A08FB1-DED1-4EC3-BECF-606C3E2778AF}"/>
-    <hyperlink ref="F10" r:id="rId20" display="Kony@123" xr:uid="{9BF11E09-87D7-49E4-88D0-6BA6B40BBDB2}"/>
-    <hyperlink ref="F11" r:id="rId21" display="Kony@123" xr:uid="{0B13BDA1-92A3-40B9-B600-C680436BCB46}"/>
-    <hyperlink ref="F12" r:id="rId22" display="Kony@123" xr:uid="{A4B2AA20-AE85-401E-A4AC-DA2C8B85C069}"/>
-    <hyperlink ref="F13" r:id="rId23" display="Kony@123" xr:uid="{E694F999-DB4A-4E16-877A-0197AA295A6A}"/>
-    <hyperlink ref="F14" r:id="rId24" display="Kony@123" xr:uid="{9BEF8D2A-97FD-4D7C-A4E5-98F01BF31502}"/>
-    <hyperlink ref="F15" r:id="rId25" display="Kony@123" xr:uid="{64F7CE5A-4CB1-4C67-9582-D17D5ED8E4FE}"/>
-    <hyperlink ref="F18" r:id="rId26" display="Kony@123" xr:uid="{72D49926-85B3-4C08-9510-37BFEB7B489B}"/>
-    <hyperlink ref="F19" r:id="rId27" display="Kony@123" xr:uid="{87866760-2DB7-4039-B9C4-E96B865E9395}"/>
-    <hyperlink ref="F21" r:id="rId28" display="Kony@123" xr:uid="{F0653554-2308-48C5-9404-CB9C6D8A6B0C}"/>
-    <hyperlink ref="F22" r:id="rId29" display="Kony@123" xr:uid="{DF2C3F7B-EB99-4939-B8C2-8139B4A0B6E5}"/>
-    <hyperlink ref="F23" r:id="rId30" display="Kony@123" xr:uid="{3C98B11D-26F3-4FF1-8696-87BC8FE432DE}"/>
-    <hyperlink ref="F24" r:id="rId31" display="Kony@123" xr:uid="{F50DD16B-F3EF-41E8-916F-71185B9FC64C}"/>
-    <hyperlink ref="F25" r:id="rId32" display="Kony@123" xr:uid="{B820EB0C-6373-4A55-ACDA-16C9426E2360}"/>
-    <hyperlink ref="F26" r:id="rId33" display="Kony@123" xr:uid="{7FE49DA8-FD83-4B46-BF77-2F18B4F36EF9}"/>
-    <hyperlink ref="F27" r:id="rId34" display="Kony@123" xr:uid="{63AD937C-79A8-4971-814E-42CAF285E6FD}"/>
-    <hyperlink ref="F28" r:id="rId35" display="Kony@123" xr:uid="{60968FFA-A588-4D1E-AC4F-954F10C56AF3}"/>
-    <hyperlink ref="F29" r:id="rId36" display="Kony@123" xr:uid="{B15B5200-1276-4AA8-89D7-43A9197D41AF}"/>
-    <hyperlink ref="F30" r:id="rId37" display="Kony@123" xr:uid="{57BBCCD0-13DB-43BB-B028-F36F8CC317CC}"/>
-    <hyperlink ref="F31" r:id="rId38" display="Kony@123" xr:uid="{23BC9856-CB23-48C2-B1FB-E36BFDF229CE}"/>
-    <hyperlink ref="F32" r:id="rId39" display="Kony@123" xr:uid="{1014470F-0051-4145-A480-6F738A91D1B0}"/>
-    <hyperlink ref="F33" r:id="rId40" display="Kony@123" xr:uid="{9563D07C-7B00-4285-A678-F0388C4AAC6C}"/>
-    <hyperlink ref="F43" r:id="rId41" display="Kony@123" xr:uid="{112CF6B3-0086-45DB-B506-305E30DD5F33}"/>
-    <hyperlink ref="F44" r:id="rId42" display="Kony@123" xr:uid="{A6FFE977-C3AC-449E-A3F1-35E8ECC18243}"/>
-    <hyperlink ref="F45" r:id="rId43" display="Kony@123" xr:uid="{20BFF49F-3D9E-4DA3-B0B4-3EDBB6DF93F1}"/>
-    <hyperlink ref="F46" r:id="rId44" display="Kony@123" xr:uid="{CD82CA82-782B-4594-AC15-19544D9F9C8B}"/>
-    <hyperlink ref="F47" r:id="rId45" display="Kony@123" xr:uid="{38A7D0DD-DE6E-4293-8E02-C74B6526F10B}"/>
-    <hyperlink ref="F48" r:id="rId46" display="Kony@123" xr:uid="{F21DF479-80D7-4875-A66D-72DA5E449D30}"/>
-    <hyperlink ref="F49" r:id="rId47" display="Kony@123" xr:uid="{C43106AF-CE48-4D4D-9F44-4B220B53DECE}"/>
-    <hyperlink ref="F50" r:id="rId48" display="Kony@123" xr:uid="{CA6EFCAE-911B-47E9-BF2E-DAA2209E7A71}"/>
-    <hyperlink ref="F51" r:id="rId49" display="Kony@123" xr:uid="{09570598-1CCC-470F-8A5E-6801A155BFF0}"/>
-    <hyperlink ref="F52" r:id="rId50" display="Kony@123" xr:uid="{38F26C89-EBE2-46F3-98BB-1A7378135234}"/>
-    <hyperlink ref="F53" r:id="rId51" display="Kony@123" xr:uid="{1686E96D-707F-4A18-ACA6-935646170B3D}"/>
-    <hyperlink ref="F54" r:id="rId52" display="Kony@123" xr:uid="{1619FB29-A79D-4E6B-B4A2-D956D14FAC45}"/>
-    <hyperlink ref="F55" r:id="rId53" display="Kony@123" xr:uid="{CE7CEF5D-E058-4C89-94D7-99A6CDE97CB3}"/>
-    <hyperlink ref="F56" r:id="rId54" display="Kony@123" xr:uid="{2EDE3577-F6A7-4F5B-AFB7-BC92AC6F59AF}"/>
-    <hyperlink ref="F57" r:id="rId55" display="Kony@123" xr:uid="{81F5DA1F-7FFF-4B4C-9928-6F3302B1E637}"/>
-    <hyperlink ref="F58" r:id="rId56" display="Kony@123" xr:uid="{73E4B230-6257-45E3-978D-06EBE2261946}"/>
-    <hyperlink ref="F59" r:id="rId57" display="Kony@123" xr:uid="{AC08AD28-BE28-49AD-B4D5-45164A26DEA5}"/>
-    <hyperlink ref="F60" r:id="rId58" display="Kony@123" xr:uid="{4AE8FEBB-3253-4FE4-AF78-DCC4AF8BD33C}"/>
-    <hyperlink ref="F61" r:id="rId59" display="Kony@123" xr:uid="{15218EE4-B510-40F6-B18B-2A01E2F3EC7E}"/>
-    <hyperlink ref="F62" r:id="rId60" display="Kony@123" xr:uid="{A249844A-EFD7-4C54-84B3-52CAB7B2E8E5}"/>
-    <hyperlink ref="F63" r:id="rId61" display="Kony@123" xr:uid="{1A963F5C-5948-4203-8AAD-2A5B688A7E3D}"/>
-    <hyperlink ref="F64" r:id="rId62" display="Kony@123" xr:uid="{72A376C6-204F-4076-9667-E94EB401CAA0}"/>
-    <hyperlink ref="F65" r:id="rId63" display="Kony@123" xr:uid="{3B0DFB31-690D-4922-BF6E-E1EA30C36A51}"/>
-    <hyperlink ref="F66" r:id="rId64" display="Kony@123" xr:uid="{57A0819C-2069-4906-BA64-16F8BA866D9D}"/>
-    <hyperlink ref="F67" r:id="rId65" display="Kony@123" xr:uid="{49690EA3-8504-4FDE-97F0-61DC470952BA}"/>
-    <hyperlink ref="F68" r:id="rId66" display="Kony@123" xr:uid="{EEBB06B6-9044-406C-A3A1-99B83FABCADC}"/>
-    <hyperlink ref="F69" r:id="rId67" display="Kony@123" xr:uid="{81B733E6-78EE-4E7B-8E2C-DF0B7107C340}"/>
-    <hyperlink ref="F70" r:id="rId68" display="Kony@123" xr:uid="{0082AC9D-7E42-43B9-9BC7-669DF312F639}"/>
-    <hyperlink ref="F71" r:id="rId69" display="Kony@123" xr:uid="{20E7F5E7-FD1D-4162-B621-BD95048B4766}"/>
-    <hyperlink ref="F72" r:id="rId70" display="Kony@123" xr:uid="{5C90467E-B95F-4FAF-9C90-0E68CC2FE2D3}"/>
-    <hyperlink ref="F73" r:id="rId71" display="Kony@123" xr:uid="{ABBCD72D-A485-4FD5-AE43-55DE7E771213}"/>
-    <hyperlink ref="F74" r:id="rId72" display="Kony@123" xr:uid="{154490DA-872A-4FF9-B2BE-E30515995EB3}"/>
-    <hyperlink ref="F75" r:id="rId73" display="Kony@123" xr:uid="{76BC609C-5D7E-4DE9-AFA9-B69B19DAF792}"/>
-    <hyperlink ref="F76" r:id="rId74" display="Kony@123" xr:uid="{45BB160F-B547-48E0-944F-E82BBD2014AA}"/>
-    <hyperlink ref="F77" r:id="rId75" display="Kony@123" xr:uid="{967ECF78-A7CE-47D3-8E74-BCBD8059EA58}"/>
-    <hyperlink ref="F78" r:id="rId76" display="Kony@123" xr:uid="{03E8D44D-7B7B-473C-972D-22B492AC0C27}"/>
-    <hyperlink ref="F79" r:id="rId77" display="Kony@123" xr:uid="{86026426-B2A1-4AD8-8DF6-D69A61A6E8AB}"/>
-    <hyperlink ref="F80" r:id="rId78" display="Kony@123" xr:uid="{923043A5-868E-48CC-88AA-37C72D4C492B}"/>
-    <hyperlink ref="F81" r:id="rId79" display="Kony@123" xr:uid="{5CD603BC-F856-4F58-AE54-2BA8049AC162}"/>
-    <hyperlink ref="F84" r:id="rId80" display="Kony@123" xr:uid="{514ECE2E-23FA-4E59-A8C9-D45D351CF8C4}"/>
-    <hyperlink ref="F85" r:id="rId81" display="Kony@123" xr:uid="{3E9898D1-01E9-4B42-A73F-FA5D49270409}"/>
-    <hyperlink ref="F86" r:id="rId82" display="Kony@123" xr:uid="{6C8A373E-4558-4549-B5CD-3092F837F805}"/>
-    <hyperlink ref="F89" r:id="rId83" display="Kony@123" xr:uid="{5368FA05-DE10-42A6-A357-B026967FDFC0}"/>
-    <hyperlink ref="F90" r:id="rId84" display="Kony@123" xr:uid="{E1573305-91A5-4A67-B827-21F0E01814D4}"/>
-    <hyperlink ref="F91" r:id="rId85" display="Kony@123" xr:uid="{EC5310D2-FE47-42C2-977E-73FDF3CEAC7F}"/>
-    <hyperlink ref="F92" r:id="rId86" display="Kony@123" xr:uid="{5C656A0E-C03F-46A5-9750-6448B7285932}"/>
-    <hyperlink ref="F96" r:id="rId87" display="Kony@123" xr:uid="{A98E7BB1-EEC6-456A-8058-3451A27FAC90}"/>
-    <hyperlink ref="F97" r:id="rId88" display="Kony@123" xr:uid="{E3228F97-3584-4DD5-ABD2-07E68F45C80C}"/>
-    <hyperlink ref="F98" r:id="rId89" display="Kony@123" xr:uid="{6DDF2FDE-838E-4322-8C71-F3918E530CF4}"/>
-    <hyperlink ref="F99" r:id="rId90" display="Kony@123" xr:uid="{D44CA776-25FA-44A0-95CB-A5EEF1FBF3C4}"/>
-    <hyperlink ref="F100" r:id="rId91" display="Kony@123" xr:uid="{B2523F64-9756-4607-B11E-1EB609E3938F}"/>
-    <hyperlink ref="F107" r:id="rId92" display="Kony@123" xr:uid="{1B50E80F-8635-4A37-A1B8-3EFE3126D967}"/>
-    <hyperlink ref="F108" r:id="rId93" display="Kony@123" xr:uid="{C59DFF30-5C77-41E6-AC81-0C18878AC7EA}"/>
-    <hyperlink ref="F109" r:id="rId94" display="Kony@123" xr:uid="{7A5D2A42-6072-4896-9F1E-31050D9437A9}"/>
-    <hyperlink ref="F110" r:id="rId95" display="Kony@123" xr:uid="{FA658073-1F5D-4D06-92E0-380D3101CCF6}"/>
-    <hyperlink ref="F111" r:id="rId96" display="Kony@123" xr:uid="{48C8A18E-E47D-4041-9989-7071F15DA0EC}"/>
-    <hyperlink ref="F112" r:id="rId97" display="Kony@123" xr:uid="{3A0583A7-FF13-45FD-9088-EFF63FFCBCD7}"/>
-    <hyperlink ref="F113" r:id="rId98" display="Kony@123" xr:uid="{21BDCC0D-E577-4717-9003-92D0D27274D4}"/>
-    <hyperlink ref="F114" r:id="rId99" display="Kony@123" xr:uid="{E7E2F38C-536F-473A-B8DD-5C8528E5FE37}"/>
-    <hyperlink ref="F115" r:id="rId100" display="Kony@123" xr:uid="{C2E080EC-EE6D-4EBC-B2BE-24781ADB0442}"/>
-    <hyperlink ref="F116" r:id="rId101" display="Kony@123" xr:uid="{3187464A-9470-4D02-9F1E-52C4C055ECF2}"/>
-    <hyperlink ref="F117" r:id="rId102" display="Kony@123" xr:uid="{159DA2BB-A519-4242-B0EA-1C609977B49C}"/>
-    <hyperlink ref="F118" r:id="rId103" xr:uid="{52311FF1-9CF6-428D-B8C0-3A7E10D7A9D8}"/>
-    <hyperlink ref="F119" r:id="rId104" display="Kony@123" xr:uid="{31B94F7C-1214-4F06-BF23-C50F49679A20}"/>
-    <hyperlink ref="F120" r:id="rId105" display="Kony@123" xr:uid="{3BE685BC-E79E-4D92-B932-EAF4EACAC356}"/>
-    <hyperlink ref="F121" r:id="rId106" display="Kony@123" xr:uid="{E32DB1B7-A3E9-4CE2-9B76-432AD9C6A165}"/>
-    <hyperlink ref="F122" r:id="rId107" display="Kony@123" xr:uid="{F4F85C7F-8CF5-4546-A8BE-4ABB56B6C27E}"/>
-    <hyperlink ref="F123" r:id="rId108" display="Kony@123" xr:uid="{17F58A17-F652-4FE7-A79C-4C582CE9E1EE}"/>
-    <hyperlink ref="F128" r:id="rId109" display="Kony@123" xr:uid="{170A913B-DD8E-42D1-BE29-4560950D3879}"/>
-    <hyperlink ref="F129" r:id="rId110" display="Kony@123" xr:uid="{F4B90F07-77BB-46A1-9696-53FA14BE033C}"/>
-    <hyperlink ref="F130" r:id="rId111" display="Kony@123" xr:uid="{782935E3-2C87-43AE-B37F-D81167DC6C56}"/>
-    <hyperlink ref="F131" r:id="rId112" display="Kony@123" xr:uid="{46EFFD81-5FAA-4270-91E5-E92AB19C13B8}"/>
-    <hyperlink ref="F132" r:id="rId113" display="Kony@123" xr:uid="{821C6BBE-7174-4880-86C5-57EB4864C07D}"/>
-    <hyperlink ref="F124:F127" r:id="rId114" display="Kony@123" xr:uid="{609C902F-A8C4-4418-9AF6-A380CE4B9CB4}"/>
-    <hyperlink ref="F124" r:id="rId115" display="Kony@123" xr:uid="{5DBC08E0-01B2-417C-A59F-7C35CAF06534}"/>
-    <hyperlink ref="F125" r:id="rId116" display="Kony@123" xr:uid="{02499E77-EEE7-498B-AEC7-3709A2710756}"/>
-    <hyperlink ref="F126" r:id="rId117" display="Kony@123" xr:uid="{7D0F5AFC-3C66-49BE-A373-A74A3D84BA98}"/>
-    <hyperlink ref="F127" r:id="rId118" display="Kony@123" xr:uid="{2A8D54D2-DD8F-486C-9FF6-0A0567080352}"/>
-    <hyperlink ref="F93" r:id="rId119" xr:uid="{E79FD8E2-0811-4DD3-B83F-C8B1A04675C0}"/>
-    <hyperlink ref="F101" r:id="rId120" display="Kony@123" xr:uid="{E75E4D25-F5E1-4A39-8AF4-F5C3C34DF9D1}"/>
-    <hyperlink ref="F105" r:id="rId121" display="Kony@123" xr:uid="{5B762541-6788-4ECE-AE0A-1083A12FCA23}"/>
-    <hyperlink ref="F87" r:id="rId122" display="Kony@123" xr:uid="{62C1012E-874C-485C-A458-1A50D85C315E}"/>
-    <hyperlink ref="F106" r:id="rId123" display="Kony@123" xr:uid="{12217BC4-A8EF-4F82-872A-849862FE2F7B}"/>
-    <hyperlink ref="F94" r:id="rId124" display="Kony@123" xr:uid="{9673AC35-19D2-49B2-861E-4616721D221B}"/>
-    <hyperlink ref="F102" r:id="rId125" xr:uid="{0D14B215-7B6A-48D2-A6A1-3286340DEFDF}"/>
-    <hyperlink ref="F83" r:id="rId126" xr:uid="{B05A5C93-B446-44C8-9210-79F00F77CA67}"/>
-    <hyperlink ref="F88" r:id="rId127" xr:uid="{DBADFF1E-7913-4900-BF8C-A2457EF00E6E}"/>
-    <hyperlink ref="F95" r:id="rId128" xr:uid="{E8CB30C7-EED5-475A-AA4C-3BBA59D579F2}"/>
-    <hyperlink ref="F103" r:id="rId129" xr:uid="{0225E1B7-1DBD-4713-AFA3-9F849D4E1AC1}"/>
-    <hyperlink ref="F104" r:id="rId130" xr:uid="{98DE6044-3C3A-4B66-AF3A-A0BF803D4E97}"/>
+    <hyperlink ref="F20" r:id="rId1"/>
+    <hyperlink ref="F82" r:id="rId2"/>
+    <hyperlink ref="F34" r:id="rId3"/>
+    <hyperlink ref="F35" r:id="rId4"/>
+    <hyperlink ref="F36" r:id="rId5"/>
+    <hyperlink ref="F37" r:id="rId6"/>
+    <hyperlink ref="F38" r:id="rId7"/>
+    <hyperlink ref="F39" r:id="rId8"/>
+    <hyperlink ref="F40" r:id="rId9"/>
+    <hyperlink ref="F41" r:id="rId10"/>
+    <hyperlink ref="F42" r:id="rId11"/>
+    <hyperlink ref="F2" r:id="rId12" display="Kony@123"/>
+    <hyperlink ref="F3" r:id="rId13" display="Kony@123"/>
+    <hyperlink ref="F4" r:id="rId14" display="Kony@123"/>
+    <hyperlink ref="F5" r:id="rId15" display="Kony@123"/>
+    <hyperlink ref="F6" r:id="rId16" display="Kony@123"/>
+    <hyperlink ref="F7" r:id="rId17" display="Kony@123"/>
+    <hyperlink ref="F8" r:id="rId18" display="Kony@123"/>
+    <hyperlink ref="F9" r:id="rId19" display="Kony@123"/>
+    <hyperlink ref="F10" r:id="rId20" display="Kony@123"/>
+    <hyperlink ref="F11" r:id="rId21" display="Kony@123"/>
+    <hyperlink ref="F12" r:id="rId22" display="Kony@123"/>
+    <hyperlink ref="F13" r:id="rId23" display="Kony@123"/>
+    <hyperlink ref="F14" r:id="rId24" display="Kony@123"/>
+    <hyperlink ref="F15" r:id="rId25" display="Kony@123"/>
+    <hyperlink ref="F18" r:id="rId26" display="Kony@123"/>
+    <hyperlink ref="F19" r:id="rId27" display="Kony@123"/>
+    <hyperlink ref="F21" r:id="rId28" display="Kony@123"/>
+    <hyperlink ref="F22" r:id="rId29" display="Kony@123"/>
+    <hyperlink ref="F23" r:id="rId30" display="Kony@123"/>
+    <hyperlink ref="F24" r:id="rId31" display="Kony@123"/>
+    <hyperlink ref="F25" r:id="rId32" display="Kony@123"/>
+    <hyperlink ref="F26" r:id="rId33" display="Kony@123"/>
+    <hyperlink ref="F27" r:id="rId34" display="Kony@123"/>
+    <hyperlink ref="F28" r:id="rId35" display="Kony@123"/>
+    <hyperlink ref="F29" r:id="rId36" display="Kony@123"/>
+    <hyperlink ref="F30" r:id="rId37" display="Kony@123"/>
+    <hyperlink ref="F31" r:id="rId38" display="Kony@123"/>
+    <hyperlink ref="F32" r:id="rId39" display="Kony@123"/>
+    <hyperlink ref="F33" r:id="rId40" display="Kony@123"/>
+    <hyperlink ref="F43" r:id="rId41" display="Kony@123"/>
+    <hyperlink ref="F44" r:id="rId42" display="Kony@123"/>
+    <hyperlink ref="F45" r:id="rId43" display="Kony@123"/>
+    <hyperlink ref="F46" r:id="rId44" display="Kony@123"/>
+    <hyperlink ref="F47" r:id="rId45" display="Kony@123"/>
+    <hyperlink ref="F48" r:id="rId46" display="Kony@123"/>
+    <hyperlink ref="F49" r:id="rId47" display="Kony@123"/>
+    <hyperlink ref="F50" r:id="rId48" display="Kony@123"/>
+    <hyperlink ref="F51" r:id="rId49" display="Kony@123"/>
+    <hyperlink ref="F52" r:id="rId50" display="Kony@123"/>
+    <hyperlink ref="F53" r:id="rId51" display="Kony@123"/>
+    <hyperlink ref="F54" r:id="rId52" display="Kony@123"/>
+    <hyperlink ref="F55" r:id="rId53" display="Kony@123"/>
+    <hyperlink ref="F56" r:id="rId54" display="Kony@123"/>
+    <hyperlink ref="F57" r:id="rId55" display="Kony@123"/>
+    <hyperlink ref="F58" r:id="rId56" display="Kony@123"/>
+    <hyperlink ref="F59" r:id="rId57" display="Kony@123"/>
+    <hyperlink ref="F60" r:id="rId58" display="Kony@123"/>
+    <hyperlink ref="F61" r:id="rId59" display="Kony@123"/>
+    <hyperlink ref="F62" r:id="rId60" display="Kony@123"/>
+    <hyperlink ref="F63" r:id="rId61" display="Kony@123"/>
+    <hyperlink ref="F64" r:id="rId62" display="Kony@123"/>
+    <hyperlink ref="F65" r:id="rId63" display="Kony@123"/>
+    <hyperlink ref="F66" r:id="rId64" display="Kony@123"/>
+    <hyperlink ref="F67" r:id="rId65" display="Kony@123"/>
+    <hyperlink ref="F68" r:id="rId66" display="Kony@123"/>
+    <hyperlink ref="F69" r:id="rId67" display="Kony@123"/>
+    <hyperlink ref="F70" r:id="rId68" display="Kony@123"/>
+    <hyperlink ref="F71" r:id="rId69" display="Kony@123"/>
+    <hyperlink ref="F72" r:id="rId70" display="Kony@123"/>
+    <hyperlink ref="F73" r:id="rId71" display="Kony@123"/>
+    <hyperlink ref="F74" r:id="rId72" display="Kony@123"/>
+    <hyperlink ref="F75" r:id="rId73" display="Kony@123"/>
+    <hyperlink ref="F76" r:id="rId74" display="Kony@123"/>
+    <hyperlink ref="F77" r:id="rId75" display="Kony@123"/>
+    <hyperlink ref="F78" r:id="rId76" display="Kony@123"/>
+    <hyperlink ref="F79" r:id="rId77" display="Kony@123"/>
+    <hyperlink ref="F80" r:id="rId78" display="Kony@123"/>
+    <hyperlink ref="F81" r:id="rId79" display="Kony@123"/>
+    <hyperlink ref="F84" r:id="rId80" display="Kony@123"/>
+    <hyperlink ref="F85" r:id="rId81" display="Kony@123"/>
+    <hyperlink ref="F86" r:id="rId82" display="Kony@123"/>
+    <hyperlink ref="F89" r:id="rId83" display="Kony@123"/>
+    <hyperlink ref="F90" r:id="rId84" display="Kony@123"/>
+    <hyperlink ref="F91" r:id="rId85" display="Kony@123"/>
+    <hyperlink ref="F92" r:id="rId86" display="Kony@123"/>
+    <hyperlink ref="F96" r:id="rId87" display="Kony@123"/>
+    <hyperlink ref="F97" r:id="rId88" display="Kony@123"/>
+    <hyperlink ref="F98" r:id="rId89" display="Kony@123"/>
+    <hyperlink ref="F99" r:id="rId90" display="Kony@123"/>
+    <hyperlink ref="F100" r:id="rId91" display="Kony@123"/>
+    <hyperlink ref="F107" r:id="rId92" display="Kony@123"/>
+    <hyperlink ref="F108" r:id="rId93" display="Kony@123"/>
+    <hyperlink ref="F109" r:id="rId94" display="Kony@123"/>
+    <hyperlink ref="F110" r:id="rId95" display="Kony@123"/>
+    <hyperlink ref="F111" r:id="rId96" display="Kony@123"/>
+    <hyperlink ref="F112" r:id="rId97" display="Kony@123"/>
+    <hyperlink ref="F113" r:id="rId98" display="Kony@123"/>
+    <hyperlink ref="F114" r:id="rId99" display="Kony@123"/>
+    <hyperlink ref="F115" r:id="rId100" display="Kony@123"/>
+    <hyperlink ref="F116" r:id="rId101" display="Kony@123"/>
+    <hyperlink ref="F117" r:id="rId102" display="Kony@123"/>
+    <hyperlink ref="F118" r:id="rId103"/>
+    <hyperlink ref="F119" r:id="rId104" display="Kony@123"/>
+    <hyperlink ref="F120" r:id="rId105" display="Kony@123"/>
+    <hyperlink ref="F121" r:id="rId106" display="Kony@123"/>
+    <hyperlink ref="F122" r:id="rId107" display="Kony@123"/>
+    <hyperlink ref="F123" r:id="rId108" display="Kony@123"/>
+    <hyperlink ref="F128" r:id="rId109" display="Kony@123"/>
+    <hyperlink ref="F129" r:id="rId110" display="Kony@123"/>
+    <hyperlink ref="F130" r:id="rId111" display="Kony@123"/>
+    <hyperlink ref="F131" r:id="rId112" display="Kony@123"/>
+    <hyperlink ref="F132" r:id="rId113" display="Kony@123"/>
+    <hyperlink ref="F124:F127" r:id="rId114" display="Kony@123"/>
+    <hyperlink ref="F124" r:id="rId115" display="Kony@123"/>
+    <hyperlink ref="F125" r:id="rId116" display="Kony@123"/>
+    <hyperlink ref="F126" r:id="rId117" display="Kony@123"/>
+    <hyperlink ref="F127" r:id="rId118" display="Kony@123"/>
+    <hyperlink ref="F93" r:id="rId119"/>
+    <hyperlink ref="F101" r:id="rId120" display="Kony@123"/>
+    <hyperlink ref="F105" r:id="rId121" display="Kony@123"/>
+    <hyperlink ref="F87" r:id="rId122" display="Kony@123"/>
+    <hyperlink ref="F106" r:id="rId123" display="Kony@123"/>
+    <hyperlink ref="F94" r:id="rId124" display="Kony@123"/>
+    <hyperlink ref="F102" r:id="rId125"/>
+    <hyperlink ref="F83" r:id="rId126"/>
+    <hyperlink ref="F88" r:id="rId127"/>
+    <hyperlink ref="F95" r:id="rId128"/>
+    <hyperlink ref="F103" r:id="rId129"/>
+    <hyperlink ref="F104" r:id="rId130"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId131"/>
@@ -4207,7 +4217,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N42"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -4915,7 +4925,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5128,11 +5138,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H115" r:id="rId1" display="Kony@789" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="H5" r:id="rId2" xr:uid="{FAFC8C47-05E1-4C5E-8F41-BE8F346CAB9A}"/>
-    <hyperlink ref="H6" r:id="rId3" display="Kony@123" xr:uid="{9EE8056A-AEBC-48DC-B153-AFBF5EFC0A39}"/>
-    <hyperlink ref="H7" r:id="rId4" display="Kony@123" xr:uid="{EBA55935-094D-45EA-8CD4-0720D5439F75}"/>
-    <hyperlink ref="H8" r:id="rId5" display="Kony@123" xr:uid="{3EF8C29D-D7F8-4190-AAAE-C947DD1C2DF4}"/>
+    <hyperlink ref="H115" r:id="rId1" display="Kony@789"/>
+    <hyperlink ref="H5" r:id="rId2"/>
+    <hyperlink ref="H6" r:id="rId3" display="Kony@123"/>
+    <hyperlink ref="H7" r:id="rId4" display="Kony@123"/>
+    <hyperlink ref="H8" r:id="rId5" display="Kony@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -5140,7 +5150,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5222,7 +5232,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5389,11 +5399,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5572,7 +5582,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5715,7 +5725,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -6154,16 +6164,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-    <hyperlink ref="H7" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
-    <hyperlink ref="H16" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="H4" r:id="rId1"/>
+    <hyperlink ref="H7" r:id="rId2"/>
+    <hyperlink ref="H16" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6207,8 +6217,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New scripts of Q2 Automation
</commit_message>
<xml_diff>
--- a/Q2_Automation/src/main/java/com/Resources/TestData.xlsx
+++ b/Q2_Automation/src/main/java/com/Resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="781" activeTab="9"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="781" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Alerts" sheetId="8" r:id="rId8"/>
     <sheet name="Login" sheetId="9" r:id="rId9"/>
     <sheet name="cPFM" sheetId="10" r:id="rId10"/>
-    <sheet name="Sheet1" sheetId="11" r:id="rId11"/>
+    <sheet name="Transactions" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="377">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1108,6 +1108,66 @@
   </si>
   <si>
     <t>Bonus</t>
+  </si>
+  <si>
+    <t>C25160_VerifyDebtAccountDebitTransaction</t>
+  </si>
+  <si>
+    <t>C25169_VerifyAddressChangeRequestInActivityCenter</t>
+  </si>
+  <si>
+    <t>SecondAccountNumber</t>
+  </si>
+  <si>
+    <t>21941190</t>
+  </si>
+  <si>
+    <t>20082100</t>
+  </si>
+  <si>
+    <t>WorkPhone</t>
+  </si>
+  <si>
+    <t>CellPhone</t>
+  </si>
+  <si>
+    <t>56712354</t>
+  </si>
+  <si>
+    <t>67012354</t>
+  </si>
+  <si>
+    <t>C25072_VerifyQuickTransferFromAccountDashboard</t>
+  </si>
+  <si>
+    <t>C23477_VerifySecurityAlertSetupByEmail</t>
+  </si>
+  <si>
+    <t>Security Alert</t>
+  </si>
+  <si>
+    <t>Alert</t>
+  </si>
+  <si>
+    <t>C23478_VerifySecurityAlertSetupByPhoneNumber</t>
+  </si>
+  <si>
+    <t>C23404_VerifyFundTransferAboveBalanceAvailable</t>
+  </si>
+  <si>
+    <t>112102</t>
+  </si>
+  <si>
+    <t>C23409_VerifyLoanAccountNotInFromAccountDropdown</t>
+  </si>
+  <si>
+    <t>C23412_VerifyFrequencyDropdownFunctionality</t>
+  </si>
+  <si>
+    <t>Frequency dropodwn</t>
+  </si>
+  <si>
+    <t>1st day of the month,Last day of the month,1st &amp; 15th day of the month,15th &amp; last day of the month,Weekly,Every other week,Monthly,Quarterly,Semi-annually,Yearly</t>
   </si>
 </sst>
 </file>
@@ -1507,10 +1567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F152"/>
+  <dimension ref="A1:F160"/>
   <sheetViews>
-    <sheetView topLeftCell="A122" zoomScale="80" workbookViewId="0">
-      <selection activeCell="A151" sqref="A151"/>
+    <sheetView topLeftCell="A135" zoomScale="80" workbookViewId="0">
+      <selection activeCell="A163" sqref="A163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4548,6 +4608,166 @@
         <v>330</v>
       </c>
       <c r="F152" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>357</v>
+      </c>
+      <c r="B153" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C153" t="s">
+        <v>10</v>
+      </c>
+      <c r="D153" t="s">
+        <v>12</v>
+      </c>
+      <c r="E153" t="s">
+        <v>330</v>
+      </c>
+      <c r="F153" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>358</v>
+      </c>
+      <c r="B154" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C154" t="s">
+        <v>10</v>
+      </c>
+      <c r="D154" t="s">
+        <v>12</v>
+      </c>
+      <c r="E154" t="s">
+        <v>330</v>
+      </c>
+      <c r="F154" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>366</v>
+      </c>
+      <c r="B155" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C155" t="s">
+        <v>10</v>
+      </c>
+      <c r="D155" t="s">
+        <v>12</v>
+      </c>
+      <c r="E155" t="s">
+        <v>330</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>367</v>
+      </c>
+      <c r="B156" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C156" t="s">
+        <v>10</v>
+      </c>
+      <c r="D156" t="s">
+        <v>12</v>
+      </c>
+      <c r="E156" t="s">
+        <v>330</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>370</v>
+      </c>
+      <c r="B157" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C157" t="s">
+        <v>10</v>
+      </c>
+      <c r="D157" t="s">
+        <v>12</v>
+      </c>
+      <c r="E157" t="s">
+        <v>330</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>371</v>
+      </c>
+      <c r="B158" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C158" t="s">
+        <v>10</v>
+      </c>
+      <c r="D158" t="s">
+        <v>12</v>
+      </c>
+      <c r="E158" t="s">
+        <v>330</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>373</v>
+      </c>
+      <c r="B159" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C159" t="s">
+        <v>10</v>
+      </c>
+      <c r="D159" t="s">
+        <v>12</v>
+      </c>
+      <c r="E159" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F159" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>374</v>
+      </c>
+      <c r="B160" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C160" t="s">
+        <v>10</v>
+      </c>
+      <c r="D160" t="s">
+        <v>12</v>
+      </c>
+      <c r="E160" t="s">
+        <v>330</v>
+      </c>
+      <c r="F160" s="1" t="s">
         <v>312</v>
       </c>
     </row>
@@ -4703,9 +4923,17 @@
     <hyperlink ref="F150" r:id="rId148" display="Kony@123"/>
     <hyperlink ref="F151" r:id="rId149" display="Kony@123"/>
     <hyperlink ref="F152" r:id="rId150" display="Kony@123"/>
+    <hyperlink ref="F153" r:id="rId151" display="Kony@123"/>
+    <hyperlink ref="F154" r:id="rId152" display="Kony@123"/>
+    <hyperlink ref="F155" r:id="rId153" display="Kony@123"/>
+    <hyperlink ref="F156" r:id="rId154" display="Kony@123"/>
+    <hyperlink ref="F157" r:id="rId155" display="Kony@123"/>
+    <hyperlink ref="F158" r:id="rId156" display="Kony@123"/>
+    <hyperlink ref="F159" r:id="rId157" display="Kony@123"/>
+    <hyperlink ref="F160" r:id="rId158" display="Kony@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId151"/>
+  <pageSetup orientation="portrait" r:id="rId159"/>
 </worksheet>
 </file>
 
@@ -4713,8 +4941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4730,7 +4958,7 @@
       <c r="B1" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -4846,30 +5074,86 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>358</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>366</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5563,6 +5847,45 @@
       </c>
       <c r="N42" t="s">
         <v>300</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>371</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E43" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>373</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>374</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E45" t="s">
+        <v>375</v>
+      </c>
+      <c r="G45" t="s">
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -6373,10 +6696,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6807,6 +7130,17 @@
       </c>
       <c r="H16" s="1" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>367</v>
+      </c>
+      <c r="B17" t="s">
+        <v>368</v>
+      </c>
+      <c r="C17" t="s">
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ënhanced existing scripts with new changes
</commit_message>
<xml_diff>
--- a/Q2_Automation/src/main/java/com/Resources/TestData.xlsx
+++ b/Q2_Automation/src/main/java/com/Resources/TestData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Divya\git\TDECU_v6_Project_updates\TDECUProjects\Q2_Automation\src\main\java\com\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC75E98-D0C3-4BAE-9DE7-A5F1D5B7ABF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="781" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="781" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -24,20 +30,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529" uniqueCount="378">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -1168,12 +1166,15 @@
   </si>
   <si>
     <t>1st day of the month,Last day of the month,1st &amp; 15th day of the month,15th &amp; last day of the month,Weekly,Every other week,Monthly,Quarterly,Semi-annually,Yearly</t>
+  </si>
+  <si>
+    <t>Reminder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1559,18 +1560,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F160"/>
   <sheetViews>
-    <sheetView topLeftCell="A135" zoomScale="80" workbookViewId="0">
-      <selection activeCell="A163" sqref="A163"/>
+    <sheetView topLeftCell="A48" zoomScale="80" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1987,8 +1988,8 @@
       <c r="E21" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>312</v>
+      <c r="F21" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2865,7 +2866,7 @@
         <v>12</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>313</v>
+        <v>330</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>312</v>
@@ -4773,164 +4774,164 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F20" r:id="rId1"/>
-    <hyperlink ref="F82" r:id="rId2"/>
-    <hyperlink ref="F34" r:id="rId3"/>
-    <hyperlink ref="F35" r:id="rId4"/>
-    <hyperlink ref="F36" r:id="rId5"/>
-    <hyperlink ref="F37" r:id="rId6"/>
-    <hyperlink ref="F38" r:id="rId7"/>
-    <hyperlink ref="F39" r:id="rId8"/>
-    <hyperlink ref="F40" r:id="rId9"/>
-    <hyperlink ref="F41" r:id="rId10"/>
-    <hyperlink ref="F42" r:id="rId11"/>
-    <hyperlink ref="F2" r:id="rId12" display="Kony@123"/>
-    <hyperlink ref="F3" r:id="rId13" display="Kony@123"/>
-    <hyperlink ref="F4" r:id="rId14" display="Kony@123"/>
-    <hyperlink ref="F5" r:id="rId15" display="Kony@123"/>
-    <hyperlink ref="F6" r:id="rId16" display="Kony@123"/>
-    <hyperlink ref="F7" r:id="rId17" display="Kony@123"/>
-    <hyperlink ref="F8" r:id="rId18" display="Kony@123"/>
-    <hyperlink ref="F9" r:id="rId19" display="Kony@123"/>
-    <hyperlink ref="F10" r:id="rId20" display="Kony@123"/>
-    <hyperlink ref="F11" r:id="rId21" display="Kony@123"/>
-    <hyperlink ref="F12" r:id="rId22" display="Kony@123"/>
-    <hyperlink ref="F13" r:id="rId23" display="Kony@123"/>
-    <hyperlink ref="F14" r:id="rId24" display="Kony@123"/>
-    <hyperlink ref="F15" r:id="rId25" display="Kony@123"/>
-    <hyperlink ref="F18" r:id="rId26" display="Kony@123"/>
-    <hyperlink ref="F19" r:id="rId27" display="Kony@123"/>
-    <hyperlink ref="F21" r:id="rId28" display="Kony@123"/>
-    <hyperlink ref="F22" r:id="rId29" display="Kony@123"/>
-    <hyperlink ref="F23" r:id="rId30" display="Kony@123"/>
-    <hyperlink ref="F24" r:id="rId31" display="Kony@123"/>
-    <hyperlink ref="F25" r:id="rId32" display="Kony@123"/>
-    <hyperlink ref="F26" r:id="rId33" display="Kony@123"/>
-    <hyperlink ref="F27" r:id="rId34" display="Kony@123"/>
-    <hyperlink ref="F28" r:id="rId35" display="Kony@123"/>
-    <hyperlink ref="F29" r:id="rId36" display="Kony@123"/>
-    <hyperlink ref="F30" r:id="rId37" display="Kony@123"/>
-    <hyperlink ref="F31" r:id="rId38" display="Kony@123"/>
-    <hyperlink ref="F32" r:id="rId39" display="Kony@123"/>
-    <hyperlink ref="F33" r:id="rId40" display="Kony@123"/>
-    <hyperlink ref="F43" r:id="rId41" display="Kony@123"/>
-    <hyperlink ref="F44" r:id="rId42" display="Kony@123"/>
-    <hyperlink ref="F45" r:id="rId43" display="Kony@123"/>
-    <hyperlink ref="F46" r:id="rId44" display="Kony@123"/>
-    <hyperlink ref="F47" r:id="rId45" display="Kony@123"/>
-    <hyperlink ref="F48" r:id="rId46" display="Kony@123"/>
-    <hyperlink ref="F49" r:id="rId47" display="Kony@123"/>
-    <hyperlink ref="F50" r:id="rId48" display="Kony@123"/>
-    <hyperlink ref="F51" r:id="rId49" display="Kony@123"/>
-    <hyperlink ref="F52" r:id="rId50" display="Kony@123"/>
-    <hyperlink ref="F53" r:id="rId51" display="Kony@123"/>
-    <hyperlink ref="F54" r:id="rId52" display="Kony@123"/>
-    <hyperlink ref="F55" r:id="rId53" display="Kony@123"/>
-    <hyperlink ref="F56" r:id="rId54" display="Kony@123"/>
-    <hyperlink ref="F57" r:id="rId55" display="Kony@123"/>
-    <hyperlink ref="F58" r:id="rId56" display="Kony@123"/>
-    <hyperlink ref="F59" r:id="rId57" display="Kony@123"/>
-    <hyperlink ref="F60" r:id="rId58" display="Kony@123"/>
-    <hyperlink ref="F61" r:id="rId59" display="Kony@123"/>
-    <hyperlink ref="F62" r:id="rId60" display="Kony@123"/>
-    <hyperlink ref="F63" r:id="rId61" display="Kony@123"/>
-    <hyperlink ref="F64" r:id="rId62" display="Kony@123"/>
-    <hyperlink ref="F65" r:id="rId63" display="Kony@123"/>
-    <hyperlink ref="F66" r:id="rId64" display="Kony@123"/>
-    <hyperlink ref="F67" r:id="rId65" display="Kony@123"/>
-    <hyperlink ref="F68" r:id="rId66" display="Kony@123"/>
-    <hyperlink ref="F69" r:id="rId67" display="Kony@123"/>
-    <hyperlink ref="F70" r:id="rId68" display="Kony@123"/>
-    <hyperlink ref="F71" r:id="rId69" display="Kony@123"/>
-    <hyperlink ref="F72" r:id="rId70" display="Kony@123"/>
-    <hyperlink ref="F73" r:id="rId71" display="Kony@123"/>
-    <hyperlink ref="F74" r:id="rId72" display="Kony@123"/>
-    <hyperlink ref="F75" r:id="rId73" display="Kony@123"/>
-    <hyperlink ref="F76" r:id="rId74" display="Kony@123"/>
-    <hyperlink ref="F77" r:id="rId75" display="Kony@123"/>
-    <hyperlink ref="F78" r:id="rId76" display="Kony@123"/>
-    <hyperlink ref="F79" r:id="rId77" display="Kony@123"/>
-    <hyperlink ref="F80" r:id="rId78" display="Kony@123"/>
-    <hyperlink ref="F81" r:id="rId79" display="Kony@123"/>
-    <hyperlink ref="F84" r:id="rId80" display="Kony@123"/>
-    <hyperlink ref="F85" r:id="rId81" display="Kony@123"/>
-    <hyperlink ref="F86" r:id="rId82" display="Kony@123"/>
-    <hyperlink ref="F89" r:id="rId83" display="Kony@123"/>
-    <hyperlink ref="F90" r:id="rId84" display="Kony@123"/>
-    <hyperlink ref="F91" r:id="rId85" display="Kony@123"/>
-    <hyperlink ref="F92" r:id="rId86" display="Kony@123"/>
-    <hyperlink ref="F96" r:id="rId87" display="Kony@123"/>
-    <hyperlink ref="F97" r:id="rId88" display="Kony@123"/>
-    <hyperlink ref="F98" r:id="rId89" display="Kony@123"/>
-    <hyperlink ref="F99" r:id="rId90" display="Kony@123"/>
-    <hyperlink ref="F100" r:id="rId91" display="Kony@123"/>
-    <hyperlink ref="F107" r:id="rId92" display="Kony@123"/>
-    <hyperlink ref="F108" r:id="rId93" display="Kony@123"/>
-    <hyperlink ref="F109" r:id="rId94" display="Kony@123"/>
-    <hyperlink ref="F110" r:id="rId95" display="Kony@123"/>
-    <hyperlink ref="F111" r:id="rId96" display="Kony@123"/>
-    <hyperlink ref="F112" r:id="rId97" display="Kony@123"/>
-    <hyperlink ref="F113" r:id="rId98" display="Kony@123"/>
-    <hyperlink ref="F114" r:id="rId99" display="Kony@123"/>
-    <hyperlink ref="F115" r:id="rId100" display="Kony@123"/>
-    <hyperlink ref="F116" r:id="rId101" display="Kony@123"/>
-    <hyperlink ref="F117" r:id="rId102" display="Kony@123"/>
-    <hyperlink ref="F118" r:id="rId103"/>
-    <hyperlink ref="F119" r:id="rId104" display="Kony@123"/>
-    <hyperlink ref="F120" r:id="rId105" display="Kony@123"/>
-    <hyperlink ref="F121" r:id="rId106" display="Kony@123"/>
-    <hyperlink ref="F122" r:id="rId107" display="Kony@123"/>
-    <hyperlink ref="F123" r:id="rId108" display="Kony@123"/>
-    <hyperlink ref="F128" r:id="rId109" display="Kony@123"/>
-    <hyperlink ref="F129" r:id="rId110" display="Kony@123"/>
-    <hyperlink ref="F130" r:id="rId111" display="Kony@123"/>
-    <hyperlink ref="F131" r:id="rId112" display="Kony@123"/>
-    <hyperlink ref="F132" r:id="rId113" display="Kony@123"/>
-    <hyperlink ref="F124:F127" r:id="rId114" display="Kony@123"/>
-    <hyperlink ref="F124" r:id="rId115" display="Kony@123"/>
-    <hyperlink ref="F125" r:id="rId116" display="Kony@123"/>
-    <hyperlink ref="F126" r:id="rId117" display="Kony@123"/>
-    <hyperlink ref="F127" r:id="rId118" display="Kony@123"/>
-    <hyperlink ref="F93" r:id="rId119"/>
-    <hyperlink ref="F101" r:id="rId120" display="Kony@123"/>
-    <hyperlink ref="F105" r:id="rId121" display="Kony@123"/>
-    <hyperlink ref="F87" r:id="rId122" display="Kony@123"/>
-    <hyperlink ref="F106" r:id="rId123" display="Kony@123"/>
-    <hyperlink ref="F94" r:id="rId124" display="Kony@123"/>
-    <hyperlink ref="F102" r:id="rId125"/>
-    <hyperlink ref="F83" r:id="rId126"/>
-    <hyperlink ref="F88" r:id="rId127"/>
-    <hyperlink ref="F95" r:id="rId128"/>
-    <hyperlink ref="F103" r:id="rId129"/>
-    <hyperlink ref="F104" r:id="rId130"/>
-    <hyperlink ref="F133" r:id="rId131" display="Kony@123"/>
-    <hyperlink ref="F134" r:id="rId132" display="Kony@123"/>
-    <hyperlink ref="F135" r:id="rId133" display="Kony@123"/>
-    <hyperlink ref="F136" r:id="rId134" display="Kony@123"/>
-    <hyperlink ref="F137" r:id="rId135" display="Kony@123"/>
-    <hyperlink ref="F138" r:id="rId136" display="Kony@123"/>
-    <hyperlink ref="F139" r:id="rId137" display="Kony@123"/>
-    <hyperlink ref="F140" r:id="rId138" display="Kony@123"/>
-    <hyperlink ref="F141" r:id="rId139" display="Kony@123"/>
-    <hyperlink ref="F142" r:id="rId140" display="Kony@123"/>
-    <hyperlink ref="F143" r:id="rId141" display="Kony@123"/>
-    <hyperlink ref="F144" r:id="rId142" display="Kony@123"/>
-    <hyperlink ref="F145" r:id="rId143" display="Kony@123"/>
-    <hyperlink ref="F146" r:id="rId144" display="Kony@123"/>
-    <hyperlink ref="F147" r:id="rId145" display="Kony@123"/>
-    <hyperlink ref="F148" r:id="rId146" display="Kony@123"/>
-    <hyperlink ref="F149" r:id="rId147" display="Kony@123"/>
-    <hyperlink ref="F150" r:id="rId148" display="Kony@123"/>
-    <hyperlink ref="F151" r:id="rId149" display="Kony@123"/>
-    <hyperlink ref="F152" r:id="rId150" display="Kony@123"/>
-    <hyperlink ref="F153" r:id="rId151" display="Kony@123"/>
-    <hyperlink ref="F154" r:id="rId152" display="Kony@123"/>
-    <hyperlink ref="F155" r:id="rId153" display="Kony@123"/>
-    <hyperlink ref="F156" r:id="rId154" display="Kony@123"/>
-    <hyperlink ref="F157" r:id="rId155" display="Kony@123"/>
-    <hyperlink ref="F158" r:id="rId156" display="Kony@123"/>
-    <hyperlink ref="F159" r:id="rId157" display="Kony@123"/>
-    <hyperlink ref="F160" r:id="rId158" display="Kony@123"/>
+    <hyperlink ref="F20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F82" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F34" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F35" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F36" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F37" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F38" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F39" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F40" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F41" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F42" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F2" r:id="rId12" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F3" r:id="rId13" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F4" r:id="rId14" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F5" r:id="rId15" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F6" r:id="rId16" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F7" r:id="rId17" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F8" r:id="rId18" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F9" r:id="rId19" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="F10" r:id="rId20" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="F11" r:id="rId21" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="F12" r:id="rId22" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="F13" r:id="rId23" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="F14" r:id="rId24" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="F15" r:id="rId25" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="F18" r:id="rId26" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="F19" r:id="rId27" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="F21" r:id="rId28" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="F22" r:id="rId29" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="F23" r:id="rId30" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="F24" r:id="rId31" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="F25" r:id="rId32" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="F26" r:id="rId33" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="F27" r:id="rId34" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="F28" r:id="rId35" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="F29" r:id="rId36" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="F30" r:id="rId37" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="F31" r:id="rId38" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="F32" r:id="rId39" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="F33" r:id="rId40" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="F43" r:id="rId41" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="F44" r:id="rId42" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="F45" r:id="rId43" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="F46" r:id="rId44" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="F47" r:id="rId45" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="F48" r:id="rId46" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="F49" r:id="rId47" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="F50" r:id="rId48" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="F51" r:id="rId49" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="F52" r:id="rId50" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="F53" r:id="rId51" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="F54" r:id="rId52" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="F55" r:id="rId53" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="F56" r:id="rId54" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="F57" r:id="rId55" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="F58" r:id="rId56" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="F59" r:id="rId57" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="F60" r:id="rId58" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="F61" r:id="rId59" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="F62" r:id="rId60" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="F63" r:id="rId61" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="F64" r:id="rId62" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="F65" r:id="rId63" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="F66" r:id="rId64" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="F67" r:id="rId65" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="F68" r:id="rId66" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="F69" r:id="rId67" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="F70" r:id="rId68" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="F71" r:id="rId69" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="F72" r:id="rId70" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="F73" r:id="rId71" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="F74" r:id="rId72" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="F75" r:id="rId73" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="F76" r:id="rId74" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="F77" r:id="rId75" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="F78" r:id="rId76" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="F79" r:id="rId77" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="F80" r:id="rId78" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="F81" r:id="rId79" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="F84" r:id="rId80" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="F85" r:id="rId81" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="F86" r:id="rId82" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="F89" r:id="rId83" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="F90" r:id="rId84" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="F91" r:id="rId85" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="F92" r:id="rId86" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="F96" r:id="rId87" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="F97" r:id="rId88" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="F98" r:id="rId89" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="F99" r:id="rId90" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="F100" r:id="rId91" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="F107" r:id="rId92" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="F108" r:id="rId93" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="F109" r:id="rId94" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="F110" r:id="rId95" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="F111" r:id="rId96" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="F112" r:id="rId97" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="F113" r:id="rId98" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="F114" r:id="rId99" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="F115" r:id="rId100" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="F116" r:id="rId101" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="F117" r:id="rId102" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="F118" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="F119" r:id="rId104" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="F120" r:id="rId105" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="F121" r:id="rId106" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="F122" r:id="rId107" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="F123" r:id="rId108" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="F128" r:id="rId109" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="F129" r:id="rId110" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="F130" r:id="rId111" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="F131" r:id="rId112" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="F132" r:id="rId113" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="F124:F127" r:id="rId114" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="F124" r:id="rId115" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="F125" r:id="rId116" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="F126" r:id="rId117" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="F127" r:id="rId118" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="F93" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="F101" r:id="rId120" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="F105" r:id="rId121" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="F87" r:id="rId122" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="F106" r:id="rId123" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="F94" r:id="rId124" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="F102" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="F83" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="F88" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="F95" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="F103" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="F104" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="F133" r:id="rId131" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="F134" r:id="rId132" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="F135" r:id="rId133" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="F136" r:id="rId134" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="F137" r:id="rId135" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="F138" r:id="rId136" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="F139" r:id="rId137" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="F140" r:id="rId138" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="F141" r:id="rId139" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="F142" r:id="rId140" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="F143" r:id="rId141" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="F144" r:id="rId142" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="F145" r:id="rId143" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="F146" r:id="rId144" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="F147" r:id="rId145" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="F148" r:id="rId146" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="F149" r:id="rId147" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="F150" r:id="rId148" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="F151" r:id="rId149" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="F152" r:id="rId150" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="F153" r:id="rId151" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="F154" r:id="rId152" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="F155" r:id="rId153" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="F156" r:id="rId154" display="Kony@123" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="F157" r:id="rId155" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="F158" r:id="rId156" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="F159" r:id="rId157" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="F160" r:id="rId158" display="Kony@123" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId159"/>
@@ -4938,7 +4939,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5079,7 +5080,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5148,12 +5149,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
+      <selection pane="bottomLeft" activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5895,7 +5896,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6108,11 +6109,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H115" r:id="rId1" display="Kony@789"/>
-    <hyperlink ref="H5" r:id="rId2"/>
-    <hyperlink ref="H6" r:id="rId3" display="Kony@123"/>
-    <hyperlink ref="H7" r:id="rId4" display="Kony@123"/>
-    <hyperlink ref="H8" r:id="rId5" display="Kony@123"/>
+    <hyperlink ref="H115" r:id="rId1" display="Kony@789" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="H5" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="H6" r:id="rId3" display="Kony@123" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="H7" r:id="rId4" display="Kony@123" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="H8" r:id="rId5" display="Kony@123" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
@@ -6120,7 +6121,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6202,7 +6203,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6369,7 +6370,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6552,7 +6553,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6695,11 +6696,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6790,7 +6791,7 @@
         <v>134</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>377</v>
       </c>
       <c r="C4" t="s">
         <v>124</v>
@@ -7145,16 +7146,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1"/>
-    <hyperlink ref="H7" r:id="rId2"/>
-    <hyperlink ref="H16" r:id="rId3"/>
+    <hyperlink ref="H4" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="H7" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="H16" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7198,8 +7199,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>